<commit_message>
B. de Corsi integrado y con t funcionando + Hora de Salida
</commit_message>
<xml_diff>
--- a/DAT/Exportar/Documento_Modelo/Base_de_Datos.xlsx
+++ b/DAT/Exportar/Documento_Modelo/Base_de_Datos.xlsx
@@ -769,6 +769,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -778,26 +796,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7082,10 +7082,10 @@
   <dimension ref="A1:CH6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="BS3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="BX3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BZ6" sqref="BZ6"/>
+      <selection pane="bottomRight" activeCell="CB1" sqref="CB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -7116,224 +7116,224 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:86" s="12" customFormat="1" ht="37.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="27" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="P1" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="Q1" s="27" t="s">
+      <c r="Q1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="R1" s="27" t="s">
+      <c r="R1" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="S1" s="27" t="s">
+      <c r="S1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="T1" s="27" t="s">
+      <c r="T1" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="U1" s="27" t="s">
+      <c r="U1" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="V1" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="W1" s="27" t="s">
+      <c r="W1" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="X1" s="27" t="s">
+      <c r="X1" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="Y1" s="27" t="s">
+      <c r="Y1" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="Z1" s="27" t="s">
+      <c r="Z1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="AA1" s="27" t="s">
+      <c r="AA1" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="AB1" s="27" t="s">
+      <c r="AB1" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="AC1" s="27" t="s">
+      <c r="AC1" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="AD1" s="27" t="s">
+      <c r="AD1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="AE1" s="27" t="s">
+      <c r="AE1" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="AF1" s="27" t="s">
+      <c r="AF1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="AG1" s="27" t="s">
+      <c r="AG1" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="AH1" s="27" t="s">
+      <c r="AH1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="AI1" s="27" t="s">
+      <c r="AI1" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="AJ1" s="27" t="s">
+      <c r="AJ1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="AK1" s="27" t="s">
+      <c r="AK1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="AL1" s="27" t="s">
+      <c r="AL1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="AM1" s="27" t="s">
+      <c r="AM1" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="AN1" s="27" t="s">
+      <c r="AN1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="AO1" s="27" t="s">
+      <c r="AO1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="AP1" s="27" t="s">
+      <c r="AP1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="AQ1" s="27" t="s">
+      <c r="AQ1" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="AR1" s="27" t="s">
+      <c r="AR1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="AS1" s="27" t="s">
+      <c r="AS1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="AT1" s="27" t="s">
+      <c r="AT1" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="AU1" s="27" t="s">
+      <c r="AU1" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="AV1" s="27" t="s">
+      <c r="AV1" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="AW1" s="27" t="s">
+      <c r="AW1" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="AX1" s="27" t="s">
+      <c r="AX1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="AY1" s="27" t="s">
+      <c r="AY1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="AZ1" s="27" t="s">
+      <c r="AZ1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="BA1" s="27" t="s">
+      <c r="BA1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="BB1" s="27" t="s">
+      <c r="BB1" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="BC1" s="27" t="s">
+      <c r="BC1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="BD1" s="27" t="s">
+      <c r="BD1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="BE1" s="27" t="s">
+      <c r="BE1" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="BF1" s="27" t="s">
+      <c r="BF1" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="BG1" s="27" t="s">
+      <c r="BG1" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="BH1" s="27" t="s">
+      <c r="BH1" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="BI1" s="27" t="s">
+      <c r="BI1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="BJ1" s="27" t="s">
+      <c r="BJ1" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="BK1" s="27" t="s">
+      <c r="BK1" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="BL1" s="27" t="s">
+      <c r="BL1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="BM1" s="27" t="s">
+      <c r="BM1" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="BN1" s="27" t="s">
+      <c r="BN1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="BO1" s="27" t="s">
+      <c r="BO1" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="BP1" s="27" t="s">
+      <c r="BP1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="BQ1" s="27" t="s">
+      <c r="BQ1" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="BR1" s="27" t="s">
+      <c r="BR1" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="BS1" s="27" t="s">
+      <c r="BS1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="BT1" s="27" t="s">
+      <c r="BT1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="BU1" s="27" t="s">
+      <c r="BU1" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="BV1" s="29" t="s">
+      <c r="BV1" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="BW1" s="30"/>
-      <c r="BX1" s="30"/>
-      <c r="BY1" s="30"/>
-      <c r="BZ1" s="30"/>
-      <c r="CA1" s="30"/>
+      <c r="BW1" s="27"/>
+      <c r="BX1" s="27"/>
+      <c r="BY1" s="27"/>
+      <c r="BZ1" s="27"/>
+      <c r="CA1" s="27"/>
       <c r="CB1" s="31"/>
-      <c r="CC1" s="28"/>
-      <c r="CD1" s="28"/>
-      <c r="CE1" s="28"/>
-      <c r="CF1" s="28"/>
-      <c r="CG1" s="28"/>
-      <c r="CH1" s="28"/>
+      <c r="CC1" s="23"/>
+      <c r="CD1" s="23"/>
+      <c r="CE1" s="23"/>
+      <c r="CF1" s="23"/>
+      <c r="CG1" s="23"/>
+      <c r="CH1" s="23"/>
     </row>
     <row r="2" spans="1:86" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -8147,7 +8147,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="BV1:CB1"/>
+    <mergeCell ref="BV1:CA1"/>
   </mergeCells>
   <conditionalFormatting sqref="CB3:CB4">
     <cfRule type="containsText" dxfId="163" priority="1" operator="containsText" text="R">
@@ -8302,12 +8302,12 @@
       </c>
     </row>
     <row r="3" spans="2:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="24"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
       <c r="I3" t="s">
         <v>87</v>
       </c>
@@ -8835,14 +8835,14 @@
       </c>
     </row>
     <row r="22" spans="2:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="22" t="s">
+      <c r="C22" s="30"/>
+      <c r="D22" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="E22" s="24"/>
+      <c r="E22" s="30"/>
       <c r="G22" s="11">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Intentando armar lo de Poligono. Antes de Cambiar Bloques js
</commit_message>
<xml_diff>
--- a/DAT/Exportar/Documento_Modelo/Base_de_Datos.xlsx
+++ b/DAT/Exportar/Documento_Modelo/Base_de_Datos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="194">
   <si>
     <t>ID</t>
   </si>
@@ -555,9 +555,6 @@
     <t>Max              18</t>
   </si>
   <si>
-    <t>CORSI CON INTERFERENCIA - POLÍGONOS</t>
-  </si>
-  <si>
     <t>Max                                     600.000ms</t>
   </si>
   <si>
@@ -595,6 +592,12 @@
   </si>
   <si>
     <t>Hola</t>
+  </si>
+  <si>
+    <t>Total de Series Completadas en Corsi con Interferencia</t>
+  </si>
+  <si>
+    <t>POLÍGONOS - CORSI CON INTERFERENCIA</t>
   </si>
 </sst>
 </file>
@@ -695,7 +698,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -872,17 +875,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thick">
         <color indexed="64"/>
       </left>
@@ -1217,12 +1209,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1287,12 +1316,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1305,28 +1328,31 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1335,31 +1361,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1368,7 +1391,7 @@
     <xf numFmtId="49" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1377,10 +1400,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1389,22 +1409,22 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="46" fontId="3" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="46" fontId="3" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1416,40 +1436,31 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="46" fontId="3" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="46" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1467,25 +1478,25 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1497,12 +1508,500 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="44" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Buena" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="369">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+      <numFmt numFmtId="31" formatCode="[h]:mm:ss"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color theme="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1532,485 +2031,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thick">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-      <numFmt numFmtId="31" formatCode="[h]:mm:ss"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color theme="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -8939,26 +8959,26 @@
     <tableColumn id="89" name="CS" dataDxfId="33" totalsRowDxfId="32"/>
     <tableColumn id="74" name="Serie_CS" dataDxfId="31" totalsRowDxfId="30"/>
     <tableColumn id="76" name="CI" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="88" name="Serie_CI" dataDxfId="0" totalsRowDxfId="27"/>
-    <tableColumn id="100" name="Total Series" dataDxfId="26" totalsRowDxfId="25"/>
-    <tableColumn id="101" name="Total Ensayos" dataDxfId="24" totalsRowDxfId="23">
+    <tableColumn id="88" name="Serie_CI" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="100" name="Total Series" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="101" name="Total Ensayos" dataDxfId="23" totalsRowDxfId="22">
       <calculatedColumnFormula>CH4*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="98" name="Aciertos" dataDxfId="22" totalsRowDxfId="21"/>
-    <tableColumn id="99" name="Errores" dataDxfId="20" totalsRowDxfId="19"/>
-    <tableColumn id="96" name="Vacios " dataDxfId="18" totalsRowDxfId="17"/>
-    <tableColumn id="97" name="% Acierto" dataDxfId="16" totalsRowDxfId="15">
+    <tableColumn id="98" name="Aciertos" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="99" name="Errores" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="96" name="Vacios " dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="97" name="% Acierto" dataDxfId="15" totalsRowDxfId="14">
       <calculatedColumnFormula>(CJ4/CI4)*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="87" name="RA_TR" dataDxfId="14" totalsRowDxfId="13"/>
-    <tableColumn id="86" name="RM_TR" dataDxfId="12" totalsRowDxfId="11"/>
-    <tableColumn id="85" name="RV_TR" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="91" name="CS_TR" dataDxfId="8" totalsRowDxfId="7"/>
-    <tableColumn id="90" name="CI_TR" dataDxfId="6" totalsRowDxfId="5"/>
-    <tableColumn id="93" name="Tiempo Total" dataDxfId="4" totalsRowDxfId="3">
+    <tableColumn id="87" name="RA_TR" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="86" name="RM_TR" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="85" name="RV_TR" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="91" name="CS_TR" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="90" name="CI_TR" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="93" name="Tiempo Total" dataDxfId="3" totalsRowDxfId="2">
       <calculatedColumnFormula>A4-BZ4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="80" name="¿Abandonó?" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="80" name="¿Abandonó?" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Estilo de tabla 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9297,262 +9317,262 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:86" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="45" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="47" t="s">
+      <c r="B1" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="46" t="s">
         <v>165</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="I1" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="47" t="s">
+      <c r="J1" s="45" t="s">
         <v>153</v>
       </c>
-      <c r="K1" s="47" t="s">
+      <c r="K1" s="45" t="s">
         <v>154</v>
       </c>
-      <c r="L1" s="47" t="s">
+      <c r="L1" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="47" t="s">
+      <c r="M1" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="47" t="s">
+      <c r="N1" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="47" t="s">
+      <c r="O1" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="47" t="s">
+      <c r="P1" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="47" t="s">
+      <c r="Q1" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="47" t="s">
+      <c r="R1" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="47" t="s">
+      <c r="S1" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="47" t="s">
+      <c r="T1" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="47" t="s">
+      <c r="U1" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="47" t="s">
+      <c r="V1" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="W1" s="47" t="s">
+      <c r="W1" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="X1" s="47" t="s">
+      <c r="X1" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" s="47" t="s">
+      <c r="Y1" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="47" t="s">
+      <c r="Z1" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="47" t="s">
+      <c r="AA1" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" s="47" t="s">
+      <c r="AB1" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" s="47" t="s">
+      <c r="AC1" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="47" t="s">
+      <c r="AD1" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="47" t="s">
+      <c r="AE1" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="47" t="s">
+      <c r="AF1" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" s="47" t="s">
+      <c r="AG1" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" s="47" t="s">
+      <c r="AH1" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" s="47" t="s">
+      <c r="AI1" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" s="47" t="s">
+      <c r="AJ1" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="AK1" s="47" t="s">
+      <c r="AK1" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="AL1" s="47" t="s">
+      <c r="AL1" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="AM1" s="47" t="s">
+      <c r="AM1" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="AN1" s="47" t="s">
+      <c r="AN1" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="AO1" s="47" t="s">
+      <c r="AO1" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="AP1" s="47" t="s">
+      <c r="AP1" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="AQ1" s="47" t="s">
+      <c r="AQ1" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="AR1" s="47" t="s">
+      <c r="AR1" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="AS1" s="47" t="s">
+      <c r="AS1" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="AT1" s="47" t="s">
+      <c r="AT1" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="AU1" s="47" t="s">
+      <c r="AU1" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="AV1" s="47" t="s">
+      <c r="AV1" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="AW1" s="47" t="s">
+      <c r="AW1" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="AX1" s="47" t="s">
+      <c r="AX1" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="AY1" s="47" t="s">
+      <c r="AY1" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="AZ1" s="47" t="s">
+      <c r="AZ1" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="BA1" s="47" t="s">
+      <c r="BA1" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="BB1" s="47" t="s">
+      <c r="BB1" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="BC1" s="47" t="s">
+      <c r="BC1" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="BD1" s="47" t="s">
+      <c r="BD1" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="BE1" s="47" t="s">
+      <c r="BE1" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="BF1" s="47" t="s">
+      <c r="BF1" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="BG1" s="47" t="s">
+      <c r="BG1" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="BH1" s="47" t="s">
+      <c r="BH1" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="BI1" s="47" t="s">
+      <c r="BI1" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="BJ1" s="47" t="s">
+      <c r="BJ1" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="BK1" s="47" t="s">
+      <c r="BK1" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="BL1" s="47" t="s">
+      <c r="BL1" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="BM1" s="47" t="s">
+      <c r="BM1" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="BN1" s="47" t="s">
+      <c r="BN1" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="BO1" s="47" t="s">
+      <c r="BO1" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="BP1" s="47" t="s">
+      <c r="BP1" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="BQ1" s="47" t="s">
+      <c r="BQ1" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="BR1" s="47" t="s">
+      <c r="BR1" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="BS1" s="47" t="s">
+      <c r="BS1" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="BT1" s="47" t="s">
+      <c r="BT1" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="BU1" s="47" t="s">
+      <c r="BU1" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="BV1" s="47" t="s">
+      <c r="BV1" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="BW1" s="47" t="s">
+      <c r="BW1" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="BX1" s="47" t="s">
+      <c r="BX1" s="45" t="s">
         <v>156</v>
       </c>
-      <c r="BY1" s="47" t="s">
+      <c r="BY1" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="BZ1" s="47" t="s">
+      <c r="BZ1" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="CA1" s="47" t="s">
+      <c r="CA1" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="CB1" s="47" t="s">
+      <c r="CB1" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="CC1" s="47" t="s">
+      <c r="CC1" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="CD1" s="47" t="s">
+      <c r="CD1" s="45" t="s">
         <v>162</v>
       </c>
-      <c r="CE1" s="47" t="s">
+      <c r="CE1" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="CF1" s="47" t="s">
+      <c r="CF1" s="45" t="s">
         <v>164</v>
       </c>
-      <c r="CG1" s="47" t="s">
+      <c r="CG1" s="45" t="s">
         <v>167</v>
       </c>
-      <c r="CH1" s="47" t="s">
+      <c r="CH1" s="45" t="s">
         <v>151</v>
       </c>
     </row>
@@ -9567,10 +9587,10 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -9755,10 +9775,10 @@
   <dimension ref="A1:CT9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="CG4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="CH16" sqref="CH16"/>
+      <selection pane="bottomRight" activeCell="CH8" sqref="CH8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -9816,104 +9836,106 @@
       <c r="H1" s="21"/>
       <c r="I1" s="21"/>
       <c r="J1" s="17"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="27"/>
-      <c r="AR1" s="27"/>
-      <c r="AS1" s="27"/>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="27"/>
-      <c r="AV1" s="27"/>
-      <c r="AW1" s="27"/>
-      <c r="AX1" s="27"/>
-      <c r="AY1" s="27"/>
-      <c r="AZ1" s="27"/>
-      <c r="BA1" s="27"/>
-      <c r="BB1" s="27"/>
-      <c r="BC1" s="27"/>
-      <c r="BD1" s="27"/>
-      <c r="BE1" s="27"/>
-      <c r="BF1" s="29"/>
-      <c r="BG1" s="28"/>
-      <c r="BH1" s="27"/>
-      <c r="BI1" s="27"/>
-      <c r="BJ1" s="27"/>
-      <c r="BK1" s="27"/>
-      <c r="BL1" s="27"/>
-      <c r="BM1" s="27"/>
-      <c r="BN1" s="27"/>
-      <c r="BO1" s="27"/>
-      <c r="BP1" s="27"/>
-      <c r="BQ1" s="27"/>
-      <c r="BR1" s="27"/>
-      <c r="BS1" s="27"/>
-      <c r="BT1" s="27"/>
-      <c r="BU1" s="27"/>
-      <c r="BV1" s="27"/>
-      <c r="BW1" s="29"/>
-      <c r="BX1" s="77" t="s">
+      <c r="K1" s="31"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+      <c r="AJ1" s="25"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1" s="25"/>
+      <c r="AM1" s="25"/>
+      <c r="AN1" s="25"/>
+      <c r="AO1" s="25"/>
+      <c r="AP1" s="25"/>
+      <c r="AQ1" s="25"/>
+      <c r="AR1" s="25"/>
+      <c r="AS1" s="25"/>
+      <c r="AT1" s="25"/>
+      <c r="AU1" s="25"/>
+      <c r="AV1" s="25"/>
+      <c r="AW1" s="25"/>
+      <c r="AX1" s="25"/>
+      <c r="AY1" s="25"/>
+      <c r="AZ1" s="25"/>
+      <c r="BA1" s="25"/>
+      <c r="BB1" s="25"/>
+      <c r="BC1" s="25"/>
+      <c r="BD1" s="25"/>
+      <c r="BE1" s="25"/>
+      <c r="BF1" s="27"/>
+      <c r="BG1" s="26"/>
+      <c r="BH1" s="25"/>
+      <c r="BI1" s="25"/>
+      <c r="BJ1" s="25"/>
+      <c r="BK1" s="25"/>
+      <c r="BL1" s="25"/>
+      <c r="BM1" s="25"/>
+      <c r="BN1" s="25"/>
+      <c r="BO1" s="25"/>
+      <c r="BP1" s="25"/>
+      <c r="BQ1" s="25"/>
+      <c r="BR1" s="25"/>
+      <c r="BS1" s="25"/>
+      <c r="BT1" s="25"/>
+      <c r="BU1" s="25"/>
+      <c r="BV1" s="25"/>
+      <c r="BW1" s="27"/>
+      <c r="BX1" s="71" t="s">
+        <v>183</v>
+      </c>
+      <c r="BY1" s="72" t="s">
         <v>184</v>
       </c>
-      <c r="BY1" s="78" t="s">
+      <c r="BZ1" s="20"/>
+      <c r="CA1" s="76" t="s">
+        <v>182</v>
+      </c>
+      <c r="CB1" s="77"/>
+      <c r="CC1" s="77"/>
+      <c r="CD1" s="77"/>
+      <c r="CE1" s="78"/>
+      <c r="CF1" s="78"/>
+      <c r="CG1" s="79"/>
+      <c r="CH1" s="76" t="s">
+        <v>193</v>
+      </c>
+      <c r="CI1" s="77"/>
+      <c r="CJ1" s="77"/>
+      <c r="CK1" s="77"/>
+      <c r="CL1" s="78"/>
+      <c r="CM1" s="78"/>
+      <c r="CN1" s="80" t="s">
+        <v>186</v>
+      </c>
+      <c r="CO1" s="81"/>
+      <c r="CP1" s="81"/>
+      <c r="CQ1" s="81"/>
+      <c r="CR1" s="82"/>
+      <c r="CS1" s="73" t="s">
         <v>185</v>
       </c>
-      <c r="BZ1" s="20"/>
-      <c r="CA1" s="82" t="s">
-        <v>183</v>
-      </c>
-      <c r="CB1" s="83"/>
-      <c r="CC1" s="83"/>
-      <c r="CD1" s="83"/>
-      <c r="CE1" s="84"/>
-      <c r="CF1" s="84"/>
-      <c r="CG1" s="85"/>
-      <c r="CH1" s="52"/>
-      <c r="CI1" s="22"/>
-      <c r="CJ1" s="23"/>
-      <c r="CK1" s="23"/>
-      <c r="CL1" s="23"/>
-      <c r="CM1" s="23"/>
-      <c r="CN1" s="86" t="s">
-        <v>187</v>
-      </c>
-      <c r="CO1" s="87"/>
-      <c r="CP1" s="87"/>
-      <c r="CQ1" s="87"/>
-      <c r="CR1" s="88"/>
-      <c r="CS1" s="79" t="s">
-        <v>186</v>
-      </c>
-      <c r="CT1" s="80"/>
+      <c r="CT1" s="74"/>
     </row>
     <row r="2" spans="1:98" s="12" customFormat="1" ht="59.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17"/>
@@ -9926,246 +9948,246 @@
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="30" t="s">
+      <c r="K2" s="32"/>
+      <c r="L2" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="M2" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="N2" s="26" t="s">
+      <c r="N2" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="O2" s="26" t="s">
+      <c r="O2" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="P2" s="26" t="s">
+      <c r="P2" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="Q2" s="26" t="s">
+      <c r="Q2" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="R2" s="26" t="s">
+      <c r="R2" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="S2" s="26" t="s">
+      <c r="S2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="T2" s="26" t="s">
+      <c r="T2" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="U2" s="26" t="s">
+      <c r="U2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="V2" s="26" t="s">
+      <c r="V2" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="W2" s="26" t="s">
+      <c r="W2" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="X2" s="26" t="s">
+      <c r="X2" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="Y2" s="26" t="s">
+      <c r="Y2" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="Z2" s="26" t="s">
+      <c r="Z2" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="AA2" s="26" t="s">
+      <c r="AA2" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="AB2" s="31" t="s">
+      <c r="AB2" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="AC2" s="30" t="s">
+      <c r="AC2" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="AD2" s="26" t="s">
+      <c r="AD2" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="AE2" s="26" t="s">
+      <c r="AE2" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="AF2" s="26" t="s">
+      <c r="AF2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="AG2" s="26" t="s">
+      <c r="AG2" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="AH2" s="26" t="s">
+      <c r="AH2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="AI2" s="26" t="s">
+      <c r="AI2" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="AJ2" s="26" t="s">
+      <c r="AJ2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="AK2" s="26" t="s">
+      <c r="AK2" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="AL2" s="26" t="s">
+      <c r="AL2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="AM2" s="26" t="s">
+      <c r="AM2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="AN2" s="26" t="s">
+      <c r="AN2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="AO2" s="26" t="s">
+      <c r="AO2" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="AP2" s="26" t="s">
+      <c r="AP2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="AQ2" s="26" t="s">
+      <c r="AQ2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="AR2" s="26" t="s">
+      <c r="AR2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="AS2" s="26" t="s">
+      <c r="AS2" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="AT2" s="26" t="s">
+      <c r="AT2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="AU2" s="26" t="s">
+      <c r="AU2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="AV2" s="26" t="s">
+      <c r="AV2" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="AW2" s="26" t="s">
+      <c r="AW2" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="AX2" s="26" t="s">
+      <c r="AX2" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="AY2" s="26" t="s">
+      <c r="AY2" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="AZ2" s="26" t="s">
+      <c r="AZ2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="BA2" s="26" t="s">
+      <c r="BA2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="BB2" s="26" t="s">
+      <c r="BB2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="BC2" s="26" t="s">
+      <c r="BC2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="BD2" s="26" t="s">
+      <c r="BD2" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="BE2" s="26" t="s">
+      <c r="BE2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="BF2" s="31" t="s">
+      <c r="BF2" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="BG2" s="30" t="s">
+      <c r="BG2" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="BH2" s="26" t="s">
+      <c r="BH2" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="BI2" s="26" t="s">
+      <c r="BI2" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="BJ2" s="26" t="s">
+      <c r="BJ2" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="BK2" s="26" t="s">
+      <c r="BK2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="BL2" s="26" t="s">
+      <c r="BL2" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="BM2" s="26" t="s">
+      <c r="BM2" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="BN2" s="26" t="s">
+      <c r="BN2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="BO2" s="26" t="s">
+      <c r="BO2" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="BP2" s="26" t="s">
+      <c r="BP2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="BQ2" s="26" t="s">
+      <c r="BQ2" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="BR2" s="26" t="s">
+      <c r="BR2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="BS2" s="26" t="s">
+      <c r="BS2" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="BT2" s="26" t="s">
+      <c r="BT2" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="BU2" s="26" t="s">
+      <c r="BU2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="BV2" s="26" t="s">
+      <c r="BV2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="BW2" s="31" t="s">
+      <c r="BW2" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="BX2" s="77"/>
-      <c r="BY2" s="78"/>
+      <c r="BX2" s="71"/>
+      <c r="BY2" s="72"/>
       <c r="BZ2" s="19"/>
-      <c r="CA2" s="49" t="s">
+      <c r="CA2" s="47" t="s">
         <v>174</v>
       </c>
-      <c r="CB2" s="50" t="s">
+      <c r="CB2" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="CC2" s="50" t="s">
+      <c r="CC2" s="48" t="s">
         <v>176</v>
       </c>
-      <c r="CD2" s="50" t="s">
+      <c r="CD2" s="48" t="s">
         <v>177</v>
       </c>
-      <c r="CE2" s="51" t="s">
+      <c r="CE2" s="49" t="s">
+        <v>189</v>
+      </c>
+      <c r="CF2" s="49" t="s">
+        <v>178</v>
+      </c>
+      <c r="CG2" s="55" t="s">
         <v>190</v>
       </c>
-      <c r="CF2" s="51" t="s">
-        <v>178</v>
-      </c>
-      <c r="CG2" s="58" t="s">
-        <v>191</v>
-      </c>
-      <c r="CH2" s="72" t="s">
+      <c r="CH2" s="88" t="s">
+        <v>192</v>
+      </c>
+      <c r="CI2" s="86"/>
+      <c r="CJ2" s="86"/>
+      <c r="CK2" s="86"/>
+      <c r="CL2" s="86"/>
+      <c r="CM2" s="87"/>
+      <c r="CN2" s="50" t="s">
         <v>179</v>
       </c>
-      <c r="CI2" s="73"/>
-      <c r="CJ2" s="73"/>
-      <c r="CK2" s="73"/>
-      <c r="CL2" s="73"/>
-      <c r="CM2" s="74"/>
-      <c r="CN2" s="53" t="s">
+      <c r="CO2" s="51" t="s">
         <v>180</v>
       </c>
-      <c r="CO2" s="54" t="s">
+      <c r="CP2" s="51" t="s">
+        <v>179</v>
+      </c>
+      <c r="CQ2" s="69" t="s">
         <v>181</v>
       </c>
-      <c r="CP2" s="54" t="s">
-        <v>180</v>
-      </c>
-      <c r="CQ2" s="75" t="s">
-        <v>182</v>
-      </c>
-      <c r="CR2" s="76"/>
-      <c r="CS2" s="81"/>
-      <c r="CT2" s="80"/>
+      <c r="CR2" s="70"/>
+      <c r="CS2" s="75"/>
+      <c r="CT2" s="74"/>
     </row>
     <row r="3" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
@@ -10249,7 +10271,7 @@
       <c r="AA3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="AB3" s="32" t="s">
+      <c r="AB3" s="30" t="s">
         <v>23</v>
       </c>
       <c r="AC3" s="16" t="s">
@@ -10339,7 +10361,7 @@
       <c r="BE3" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="BF3" s="32" t="s">
+      <c r="BF3" s="30" t="s">
         <v>53</v>
       </c>
       <c r="BG3" s="16" t="s">
@@ -10390,13 +10412,13 @@
       <c r="BV3" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="BW3" s="32" t="s">
+      <c r="BW3" s="30" t="s">
         <v>70</v>
       </c>
       <c r="BX3" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="BY3" s="32" t="s">
+      <c r="BY3" s="30" t="s">
         <v>157</v>
       </c>
       <c r="BZ3" s="18" t="s">
@@ -10415,13 +10437,13 @@
         <v>159</v>
       </c>
       <c r="CE3" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="CF3" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="CG3" s="59" t="s">
-        <v>189</v>
+      <c r="CG3" s="56" t="s">
+        <v>188</v>
       </c>
       <c r="CH3" s="13" t="s">
         <v>168</v>
@@ -10441,604 +10463,604 @@
       <c r="CM3" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="CN3" s="60" t="s">
+      <c r="CN3" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="CO3" s="61" t="s">
+      <c r="CO3" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="CP3" s="61" t="s">
+      <c r="CP3" s="58" t="s">
         <v>73</v>
       </c>
       <c r="CQ3" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="CR3" s="24" t="s">
+      <c r="CR3" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="CS3" s="25" t="s">
+      <c r="CS3" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="CT3" s="24" t="s">
+      <c r="CT3" s="22" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:98" x14ac:dyDescent="0.3">
-      <c r="A4" s="62"/>
-      <c r="B4" s="63"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63"/>
-      <c r="J4" s="63"/>
-      <c r="K4" s="63"/>
-      <c r="L4" s="65">
+      <c r="A4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="62">
         <f>IF(Original!L2 = Corrección!$L$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="M4" s="63">
+      <c r="M4" s="60">
         <f>IF(Original!M2 = Corrección!$M$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="N4" s="63">
+      <c r="N4" s="60">
         <f>IF(Original!N2 = Corrección!$N$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="O4" s="63">
+      <c r="O4" s="60">
         <f>IF(Original!O2 = Corrección!$O$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="P4" s="63">
+      <c r="P4" s="60">
         <f>IF(Original!P2 = Corrección!$P$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="63">
+      <c r="Q4" s="60">
         <f>IF(Original!Q2 = Corrección!$Q$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="R4" s="63">
+      <c r="R4" s="60">
         <f>IF(Original!R2 = Corrección!$R$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="S4" s="63">
+      <c r="S4" s="60">
         <f>IF(Original!S2 = Corrección!$S$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="T4" s="63">
+      <c r="T4" s="60">
         <f>IF(Original!T2 = Corrección!$T$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="U4" s="63">
+      <c r="U4" s="60">
         <f>IF(Original!U2 = Corrección!$U$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="V4" s="63">
+      <c r="V4" s="60">
         <f>IF(Original!V2 = Corrección!$V$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="W4" s="63">
+      <c r="W4" s="60">
         <f>IF(Original!W2 = Corrección!$W$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="X4" s="63">
+      <c r="X4" s="60">
         <f>IF(Original!X2 = Corrección!$X$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Y4" s="63">
+      <c r="Y4" s="60">
         <f>IF(Original!Y2 = Corrección!$Y$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Z4" s="63">
+      <c r="Z4" s="60">
         <f>IF(Original!Z2 = Corrección!$Z$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AA4" s="63">
+      <c r="AA4" s="60">
         <f>IF(Original!AA2 = Corrección!$AA$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AB4" s="66">
+      <c r="AB4" s="63">
         <f>IF(Original!AB2 = Corrección!$AB$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AC4" s="65">
+      <c r="AC4" s="62">
         <f>IF(Original!AC2 = Corrección!$AC$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AD4" s="63">
+      <c r="AD4" s="60">
         <f>IF(Original!AD2 = Corrección!$AD$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AE4" s="63">
+      <c r="AE4" s="60">
         <f>IF(Original!AE2 = Corrección!$AE$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AF4" s="63">
+      <c r="AF4" s="60">
         <f>IF(Original!AF2 = Corrección!$AF$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AG4" s="63">
+      <c r="AG4" s="60">
         <f>IF(Original!AG2 = Corrección!$AG$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AH4" s="63">
+      <c r="AH4" s="60">
         <f>IF(Original!AH2 = Corrección!$AH$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AI4" s="63">
+      <c r="AI4" s="60">
         <f>IF(Original!AI2 = Corrección!$AI$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AJ4" s="63">
+      <c r="AJ4" s="60">
         <f>IF(Original!AJ2 = Corrección!$AJ$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AK4" s="63">
+      <c r="AK4" s="60">
         <f>IF(Original!AK2 = Corrección!$AK$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AL4" s="63">
+      <c r="AL4" s="60">
         <f>IF(Original!AL2 = Corrección!$AL$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AM4" s="63">
+      <c r="AM4" s="60">
         <f>IF(Original!AM2 = Corrección!$AM$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AN4" s="63">
+      <c r="AN4" s="60">
         <f>IF(Original!AN2 = Corrección!$AN$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AO4" s="63">
+      <c r="AO4" s="60">
         <f>IF(Original!AO2 = Corrección!$AO$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AP4" s="63">
+      <c r="AP4" s="60">
         <f>IF(Original!AP2 = Corrección!$AP$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AQ4" s="63">
+      <c r="AQ4" s="60">
         <f>IF(Original!AQ2 = Corrección!$AQ$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AR4" s="63">
+      <c r="AR4" s="60">
         <f>IF(Original!AR2 = Corrección!$AR$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AS4" s="63">
+      <c r="AS4" s="60">
         <f>IF(Original!AS2 = Corrección!$AS$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AT4" s="63">
+      <c r="AT4" s="60">
         <f>IF(Original!AT2 = Corrección!$AT$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AU4" s="63">
+      <c r="AU4" s="60">
         <f>IF(Original!AU2 = Corrección!$AU$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AV4" s="63">
+      <c r="AV4" s="60">
         <f>IF(Original!AV2 = Corrección!$AV$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AW4" s="63">
+      <c r="AW4" s="60">
         <f>IF(Original!AW2 = Corrección!$AW$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AX4" s="63">
+      <c r="AX4" s="60">
         <f>IF(Original!AX2 = Corrección!$AX$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AY4" s="63">
+      <c r="AY4" s="60">
         <f>IF(Original!AY2 = Corrección!$AY$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AZ4" s="63">
+      <c r="AZ4" s="60">
         <f>IF(Original!AZ2 = Corrección!$AZ$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BA4" s="63">
+      <c r="BA4" s="60">
         <f>IF(Original!BA2 = Corrección!$BA$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BB4" s="63">
+      <c r="BB4" s="60">
         <f>IF(Original!BB2 = Corrección!$BB$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BC4" s="63">
+      <c r="BC4" s="60">
         <f>IF(Original!BC2 = Corrección!$BC$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BD4" s="63">
+      <c r="BD4" s="60">
         <f>IF(Original!BD2 = Corrección!$BD$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BE4" s="63">
+      <c r="BE4" s="60">
         <f>IF(Original!BE2 = Corrección!$BE$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BF4" s="66">
+      <c r="BF4" s="63">
         <f>IF(Original!BF2 = Corrección!$BF$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BG4" s="65">
+      <c r="BG4" s="62">
         <f>IF(Original!BG2 = Corrección!$BG$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BH4" s="63">
+      <c r="BH4" s="60">
         <f>IF(Original!BH2 = Corrección!$BH$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BI4" s="63">
+      <c r="BI4" s="60">
         <f>IF(Original!BI2 = Corrección!$BI$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BJ4" s="63">
+      <c r="BJ4" s="60">
         <f>IF(Original!BJ2 = Corrección!$BJ$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BK4" s="63">
+      <c r="BK4" s="60">
         <f>IF(Original!BK2 = Corrección!$BK$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BL4" s="63">
+      <c r="BL4" s="60">
         <f>IF(Original!BL2 = Corrección!$BL$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BM4" s="63">
+      <c r="BM4" s="60">
         <f>IF(Original!BM2 = Corrección!$BM$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BN4" s="63">
+      <c r="BN4" s="60">
         <f>IF(Original!BN2 = Corrección!$BN$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BO4" s="63">
+      <c r="BO4" s="60">
         <f>IF(Original!BO2 = Corrección!$BO$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BP4" s="63">
+      <c r="BP4" s="60">
         <f>IF(Original!BP2 = Corrección!$BP$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BQ4" s="63">
+      <c r="BQ4" s="60">
         <f>IF(Original!BQ2 = Corrección!$BQ$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BR4" s="63">
+      <c r="BR4" s="60">
         <f>IF(Original!BR2 = Corrección!$BR$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BS4" s="63">
+      <c r="BS4" s="60">
         <f>IF(Original!BS2 = Corrección!$BS$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BT4" s="63">
+      <c r="BT4" s="60">
         <f>IF(Original!BT2 = Corrección!$BT$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BU4" s="63">
+      <c r="BU4" s="60">
         <f>IF(Original!BU2 = Corrección!$BU$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BV4" s="63">
+      <c r="BV4" s="60">
         <f>IF(Original!BV2 = Corrección!$BV$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BW4" s="66">
+      <c r="BW4" s="63">
         <f>IF(Original!BW2 = Corrección!$BW$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BX4" s="65"/>
-      <c r="BY4" s="66"/>
-      <c r="BZ4" s="67"/>
-      <c r="CA4" s="65">
+      <c r="BX4" s="62"/>
+      <c r="BY4" s="63"/>
+      <c r="BZ4" s="64"/>
+      <c r="CA4" s="62">
         <f t="shared" ref="CA4" si="0">SUM(L4:AB4)</f>
         <v>0</v>
       </c>
-      <c r="CB4" s="63">
+      <c r="CB4" s="60">
         <f t="shared" ref="CB4" si="1">SUM(AC4:BF4)</f>
         <v>0</v>
       </c>
-      <c r="CC4" s="63">
+      <c r="CC4" s="60">
         <f t="shared" ref="CC4:CC5" si="2">SUM(BG4:BW4)</f>
         <v>0</v>
       </c>
-      <c r="CD4" s="63"/>
-      <c r="CE4" s="63"/>
-      <c r="CF4" s="63"/>
-      <c r="CG4" s="68"/>
-      <c r="CH4" s="63">
+      <c r="CD4" s="60"/>
+      <c r="CE4" s="60"/>
+      <c r="CF4" s="60"/>
+      <c r="CG4" s="65"/>
+      <c r="CH4" s="60">
         <v>1</v>
       </c>
-      <c r="CI4" s="63">
+      <c r="CI4" s="60">
         <f>CH4*3</f>
         <v>3</v>
       </c>
-      <c r="CJ4" s="63">
-        <v>0</v>
-      </c>
-      <c r="CK4" s="63"/>
-      <c r="CL4" s="63"/>
-      <c r="CM4" s="69">
+      <c r="CJ4" s="60">
+        <v>0</v>
+      </c>
+      <c r="CK4" s="60"/>
+      <c r="CL4" s="60"/>
+      <c r="CM4" s="66">
         <f t="shared" ref="CM4:CM5" si="3">(CJ4/CI4)*100</f>
         <v>0</v>
       </c>
-      <c r="CN4" s="70"/>
-      <c r="CO4" s="63"/>
-      <c r="CP4" s="63"/>
-      <c r="CQ4" s="63"/>
-      <c r="CR4" s="63"/>
-      <c r="CS4" s="71">
+      <c r="CN4" s="67"/>
+      <c r="CO4" s="60"/>
+      <c r="CP4" s="60"/>
+      <c r="CQ4" s="60"/>
+      <c r="CR4" s="60"/>
+      <c r="CS4" s="68">
         <f t="shared" ref="CS4:CS5" si="4">A4-BZ4</f>
         <v>0</v>
       </c>
-      <c r="CT4" s="66"/>
+      <c r="CT4" s="63"/>
     </row>
     <row r="5" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
-      <c r="L5" s="36">
+      <c r="L5" s="34">
         <f>IF(Original!L3 = Corrección!$L$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="M5" s="37">
+      <c r="M5" s="35">
         <f>IF(Original!M3 = Corrección!$M$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="N5" s="37">
+      <c r="N5" s="35">
         <f>IF(Original!N3 = Corrección!$N$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="O5" s="37">
+      <c r="O5" s="35">
         <f>IF(Original!O3 = Corrección!$O$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="P5" s="37">
+      <c r="P5" s="35">
         <f>IF(Original!P3 = Corrección!$P$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="37">
+      <c r="Q5" s="35">
         <f>IF(Original!Q3 = Corrección!$Q$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="R5" s="37">
+      <c r="R5" s="35">
         <f>IF(Original!R3 = Corrección!$R$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="S5" s="37">
+      <c r="S5" s="35">
         <f>IF(Original!S3 = Corrección!$S$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="T5" s="37">
+      <c r="T5" s="35">
         <f>IF(Original!T3 = Corrección!$T$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="U5" s="37">
+      <c r="U5" s="35">
         <f>IF(Original!U3 = Corrección!$U$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="V5" s="37">
+      <c r="V5" s="35">
         <f>IF(Original!V3 = Corrección!$V$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="W5" s="37">
+      <c r="W5" s="35">
         <f>IF(Original!W3 = Corrección!$W$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="X5" s="37">
+      <c r="X5" s="35">
         <f>IF(Original!X3 = Corrección!$X$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Y5" s="37">
+      <c r="Y5" s="35">
         <f>IF(Original!Y3 = Corrección!$Y$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Z5" s="37">
+      <c r="Z5" s="35">
         <f>IF(Original!Z3 = Corrección!$Z$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AA5" s="37">
+      <c r="AA5" s="35">
         <f>IF(Original!AA3 = Corrección!$AA$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AB5" s="38">
+      <c r="AB5" s="36">
         <f>IF(Original!AB3 = Corrección!$AB$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AC5" s="36">
+      <c r="AC5" s="34">
         <f>IF(Original!AC3 = Corrección!$AC$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AD5" s="37">
+      <c r="AD5" s="35">
         <f>IF(Original!AD3 = Corrección!$AD$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AE5" s="37">
+      <c r="AE5" s="35">
         <f>IF(Original!AE3 = Corrección!$AE$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AF5" s="37">
+      <c r="AF5" s="35">
         <f>IF(Original!AF3 = Corrección!$AF$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AG5" s="37">
+      <c r="AG5" s="35">
         <f>IF(Original!AG3 = Corrección!$AG$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AH5" s="37">
+      <c r="AH5" s="35">
         <f>IF(Original!AH3 = Corrección!$AH$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AI5" s="37">
+      <c r="AI5" s="35">
         <f>IF(Original!AI3 = Corrección!$AI$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AJ5" s="37">
+      <c r="AJ5" s="35">
         <f>IF(Original!AJ3 = Corrección!$AJ$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AK5" s="37">
+      <c r="AK5" s="35">
         <f>IF(Original!AK3 = Corrección!$AK$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AL5" s="37">
+      <c r="AL5" s="35">
         <f>IF(Original!AL3 = Corrección!$AL$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AM5" s="37">
+      <c r="AM5" s="35">
         <f>IF(Original!AM3 = Corrección!$AM$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AN5" s="39">
+      <c r="AN5" s="37">
         <f>IF(Original!AN3 = Corrección!$AN$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AO5" s="39">
+      <c r="AO5" s="37">
         <f>IF(Original!AO3 = Corrección!$AO$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AP5" s="39">
+      <c r="AP5" s="37">
         <f>IF(Original!AP3 = Corrección!$AP$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AQ5" s="39">
+      <c r="AQ5" s="37">
         <f>IF(Original!AQ3 = Corrección!$AQ$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AR5" s="39">
+      <c r="AR5" s="37">
         <f>IF(Original!AR3 = Corrección!$AR$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AS5" s="39">
+      <c r="AS5" s="37">
         <f>IF(Original!AS3 = Corrección!$AS$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AT5" s="39">
+      <c r="AT5" s="37">
         <f>IF(Original!AT3 = Corrección!$AT$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AU5" s="39">
+      <c r="AU5" s="37">
         <f>IF(Original!AU3 = Corrección!$AU$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AV5" s="39">
+      <c r="AV5" s="37">
         <f>IF(Original!AV3 = Corrección!$AV$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AW5" s="39">
+      <c r="AW5" s="37">
         <f>IF(Original!AW3 = Corrección!$AW$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AX5" s="39">
+      <c r="AX5" s="37">
         <f>IF(Original!AX3 = Corrección!$AX$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AY5" s="39">
+      <c r="AY5" s="37">
         <f>IF(Original!AY3 = Corrección!$AY$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AZ5" s="39">
+      <c r="AZ5" s="37">
         <f>IF(Original!AZ3 = Corrección!$AZ$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BA5" s="39">
+      <c r="BA5" s="37">
         <f>IF(Original!BA3 = Corrección!$BA$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BB5" s="39">
+      <c r="BB5" s="37">
         <f>IF(Original!BB3 = Corrección!$BB$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BC5" s="39">
+      <c r="BC5" s="37">
         <f>IF(Original!BC3 = Corrección!$BC$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BD5" s="39">
+      <c r="BD5" s="37">
         <f>IF(Original!BD3 = Corrección!$BD$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BE5" s="39">
+      <c r="BE5" s="37">
         <f>IF(Original!BE3 = Corrección!$BE$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BF5" s="40">
+      <c r="BF5" s="38">
         <f>IF(Original!BF3 = Corrección!$BF$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BG5" s="41">
+      <c r="BG5" s="39">
         <f>IF(Original!BG3 = Corrección!$BG$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BH5" s="39">
+      <c r="BH5" s="37">
         <f>IF(Original!BH3 = Corrección!$BH$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BI5" s="39">
+      <c r="BI5" s="37">
         <f>IF(Original!BI3 = Corrección!$BI$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BJ5" s="39">
+      <c r="BJ5" s="37">
         <f>IF(Original!BJ3 = Corrección!$BJ$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BK5" s="39">
+      <c r="BK5" s="37">
         <f>IF(Original!BK3 = Corrección!$BK$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BL5" s="39">
+      <c r="BL5" s="37">
         <f>IF(Original!BL3 = Corrección!$BL$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BM5" s="39">
+      <c r="BM5" s="37">
         <f>IF(Original!BM3 = Corrección!$BM$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BN5" s="39">
+      <c r="BN5" s="37">
         <f>IF(Original!BN3 = Corrección!$BN$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BO5" s="39">
+      <c r="BO5" s="37">
         <f>IF(Original!BO3 = Corrección!$BO$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BP5" s="39">
+      <c r="BP5" s="37">
         <f>IF(Original!BP3 = Corrección!$BP$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BQ5" s="39">
+      <c r="BQ5" s="37">
         <f>IF(Original!BQ3 = Corrección!$BQ$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BR5" s="39">
+      <c r="BR5" s="37">
         <f>IF(Original!BR3 = Corrección!$BR$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BS5" s="39">
+      <c r="BS5" s="37">
         <f>IF(Original!BS3 = Corrección!$BS$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BT5" s="39">
+      <c r="BT5" s="37">
         <f>IF(Original!BT3 = Corrección!$BT$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BU5" s="39">
+      <c r="BU5" s="37">
         <f>IF(Original!BU3 = Corrección!$BU$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BV5" s="39">
+      <c r="BV5" s="37">
         <f>IF(Original!BV3 = Corrección!$BV$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BW5" s="40">
+      <c r="BW5" s="38">
         <f>IF(Original!BW3 = Corrección!$BW$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BX5" s="42"/>
-      <c r="BY5" s="43"/>
-      <c r="BZ5" s="56"/>
-      <c r="CA5" s="44">
+      <c r="BX5" s="40"/>
+      <c r="BY5" s="41"/>
+      <c r="BZ5" s="53"/>
+      <c r="CA5" s="42">
         <f>SUM(L5:AB5)</f>
         <v>0</v>
       </c>
@@ -11053,7 +11075,7 @@
       <c r="CD5" s="15"/>
       <c r="CE5" s="15"/>
       <c r="CF5" s="15"/>
-      <c r="CG5" s="38"/>
+      <c r="CG5" s="36"/>
       <c r="CH5" s="15">
         <v>1</v>
       </c>
@@ -11066,20 +11088,20 @@
       </c>
       <c r="CK5" s="15"/>
       <c r="CL5" s="15"/>
-      <c r="CM5" s="55">
+      <c r="CM5" s="52">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="CN5" s="46"/>
+      <c r="CN5" s="44"/>
       <c r="CO5" s="15"/>
       <c r="CP5" s="15"/>
       <c r="CQ5" s="15"/>
       <c r="CR5" s="15"/>
-      <c r="CS5" s="57">
+      <c r="CS5" s="54">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="CT5" s="45"/>
+      <c r="CT5" s="43"/>
     </row>
     <row r="6" spans="1:98" x14ac:dyDescent="0.3">
       <c r="F6" s="4"/>
@@ -11169,7 +11191,7 @@
       <c r="CQ6" s="14"/>
       <c r="CR6" s="14"/>
       <c r="CS6" s="14"/>
-      <c r="CT6" s="35"/>
+      <c r="CT6" s="33"/>
     </row>
     <row r="7" spans="1:98" x14ac:dyDescent="0.3">
       <c r="F7" s="4"/>
@@ -11259,7 +11281,7 @@
       <c r="CQ7" s="14"/>
       <c r="CR7" s="14"/>
       <c r="CS7" s="14"/>
-      <c r="CT7" s="35"/>
+      <c r="CT7" s="33"/>
     </row>
     <row r="8" spans="1:98" x14ac:dyDescent="0.3">
       <c r="F8" s="4"/>
@@ -11279,13 +11301,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="CH2:CM2"/>
     <mergeCell ref="CQ2:CR2"/>
     <mergeCell ref="BX1:BX2"/>
     <mergeCell ref="BY1:BY2"/>
     <mergeCell ref="CS1:CT2"/>
     <mergeCell ref="CA1:CG1"/>
     <mergeCell ref="CN1:CR1"/>
+    <mergeCell ref="CH1:CM1"/>
   </mergeCells>
   <conditionalFormatting sqref="CT4:CT7">
     <cfRule type="containsText" dxfId="199" priority="1" operator="containsText" text="R">
@@ -11440,12 +11462,12 @@
       </c>
     </row>
     <row r="3" spans="2:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="83" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="91"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="85"/>
       <c r="I3" t="s">
         <v>84</v>
       </c>
@@ -11973,14 +11995,14 @@
       </c>
     </row>
     <row r="22" spans="2:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="89" t="s">
+      <c r="B22" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="91"/>
-      <c r="D22" s="89" t="s">
+      <c r="C22" s="85"/>
+      <c r="D22" s="83" t="s">
         <v>83</v>
       </c>
-      <c r="E22" s="91"/>
+      <c r="E22" s="85"/>
       <c r="G22" s="11">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Poligonos Excel Integrado y Funcionando
</commit_message>
<xml_diff>
--- a/DAT/Exportar/Documento_Modelo/Base_de_Datos.xlsx
+++ b/DAT/Exportar/Documento_Modelo/Base_de_Datos.xlsx
@@ -585,12 +585,6 @@
     <t>Serie_CI</t>
   </si>
   <si>
-    <t>Serie Alcanzada en Corsi Simple</t>
-  </si>
-  <si>
-    <t>Serie Alcanzada en Corsi con Interferencia</t>
-  </si>
-  <si>
     <t>Hola</t>
   </si>
   <si>
@@ -598,6 +592,12 @@
   </si>
   <si>
     <t>POLÍGONOS - CORSI CON INTERFERENCIA</t>
+  </si>
+  <si>
+    <t>Serie Max Alcanzada en Corsi con Interferencia   [2 a 7]</t>
+  </si>
+  <si>
+    <t>Serie Max Alcanzada en Corsi Simple      [3 a 9]</t>
   </si>
 </sst>
 </file>
@@ -1457,6 +1457,15 @@
     <xf numFmtId="46" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="44" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1507,15 +1516,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="44" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9587,10 +9587,10 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -9775,10 +9775,10 @@
   <dimension ref="A1:CT9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="CG4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="CK4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="CH8" sqref="CH8"/>
+      <selection pane="bottomRight" activeCell="CR10" sqref="CR10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -9901,43 +9901,43 @@
       <c r="BU1" s="25"/>
       <c r="BV1" s="25"/>
       <c r="BW1" s="27"/>
-      <c r="BX1" s="71" t="s">
+      <c r="BX1" s="74" t="s">
         <v>183</v>
       </c>
-      <c r="BY1" s="72" t="s">
+      <c r="BY1" s="75" t="s">
         <v>184</v>
       </c>
       <c r="BZ1" s="20"/>
-      <c r="CA1" s="76" t="s">
+      <c r="CA1" s="79" t="s">
         <v>182</v>
       </c>
-      <c r="CB1" s="77"/>
-      <c r="CC1" s="77"/>
-      <c r="CD1" s="77"/>
-      <c r="CE1" s="78"/>
-      <c r="CF1" s="78"/>
-      <c r="CG1" s="79"/>
-      <c r="CH1" s="76" t="s">
-        <v>193</v>
-      </c>
-      <c r="CI1" s="77"/>
-      <c r="CJ1" s="77"/>
-      <c r="CK1" s="77"/>
-      <c r="CL1" s="78"/>
-      <c r="CM1" s="78"/>
-      <c r="CN1" s="80" t="s">
+      <c r="CB1" s="80"/>
+      <c r="CC1" s="80"/>
+      <c r="CD1" s="80"/>
+      <c r="CE1" s="81"/>
+      <c r="CF1" s="81"/>
+      <c r="CG1" s="82"/>
+      <c r="CH1" s="79" t="s">
+        <v>191</v>
+      </c>
+      <c r="CI1" s="80"/>
+      <c r="CJ1" s="80"/>
+      <c r="CK1" s="80"/>
+      <c r="CL1" s="81"/>
+      <c r="CM1" s="81"/>
+      <c r="CN1" s="83" t="s">
         <v>186</v>
       </c>
-      <c r="CO1" s="81"/>
-      <c r="CP1" s="81"/>
-      <c r="CQ1" s="81"/>
-      <c r="CR1" s="82"/>
-      <c r="CS1" s="73" t="s">
+      <c r="CO1" s="84"/>
+      <c r="CP1" s="84"/>
+      <c r="CQ1" s="84"/>
+      <c r="CR1" s="85"/>
+      <c r="CS1" s="76" t="s">
         <v>185</v>
       </c>
-      <c r="CT1" s="74"/>
+      <c r="CT1" s="77"/>
     </row>
-    <row r="2" spans="1:98" s="12" customFormat="1" ht="59.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:98" s="12" customFormat="1" ht="78.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -10141,8 +10141,8 @@
       <c r="BW2" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="BX2" s="71"/>
-      <c r="BY2" s="72"/>
+      <c r="BX2" s="74"/>
+      <c r="BY2" s="75"/>
       <c r="BZ2" s="19"/>
       <c r="CA2" s="47" t="s">
         <v>174</v>
@@ -10157,22 +10157,22 @@
         <v>177</v>
       </c>
       <c r="CE2" s="49" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="CF2" s="49" t="s">
         <v>178</v>
       </c>
       <c r="CG2" s="55" t="s">
+        <v>192</v>
+      </c>
+      <c r="CH2" s="71" t="s">
         <v>190</v>
       </c>
-      <c r="CH2" s="88" t="s">
-        <v>192</v>
-      </c>
-      <c r="CI2" s="86"/>
-      <c r="CJ2" s="86"/>
-      <c r="CK2" s="86"/>
-      <c r="CL2" s="86"/>
-      <c r="CM2" s="87"/>
+      <c r="CI2" s="69"/>
+      <c r="CJ2" s="69"/>
+      <c r="CK2" s="69"/>
+      <c r="CL2" s="69"/>
+      <c r="CM2" s="70"/>
       <c r="CN2" s="50" t="s">
         <v>179</v>
       </c>
@@ -10182,12 +10182,12 @@
       <c r="CP2" s="51" t="s">
         <v>179</v>
       </c>
-      <c r="CQ2" s="69" t="s">
+      <c r="CQ2" s="72" t="s">
         <v>181</v>
       </c>
-      <c r="CR2" s="70"/>
-      <c r="CS2" s="75"/>
-      <c r="CT2" s="74"/>
+      <c r="CR2" s="73"/>
+      <c r="CS2" s="78"/>
+      <c r="CT2" s="77"/>
     </row>
     <row r="3" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
@@ -11462,12 +11462,12 @@
       </c>
     </row>
     <row r="3" spans="2:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="88"/>
       <c r="I3" t="s">
         <v>84</v>
       </c>
@@ -11995,14 +11995,14 @@
       </c>
     </row>
     <row r="22" spans="2:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="83" t="s">
+      <c r="B22" s="86" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="85"/>
-      <c r="D22" s="83" t="s">
+      <c r="C22" s="88"/>
+      <c r="D22" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="E22" s="85"/>
+      <c r="E22" s="88"/>
       <c r="G22" s="11">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Exportar con Bloque y Tiempo Total integrado y Funcionando. Falta Abandono
</commit_message>
<xml_diff>
--- a/DAT/Exportar/Documento_Modelo/Base_de_Datos.xlsx
+++ b/DAT/Exportar/Documento_Modelo/Base_de_Datos.xlsx
@@ -492,112 +492,112 @@
     <t>Respuesta_CI</t>
   </si>
   <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>CI</t>
+  </si>
+  <si>
+    <t>CS_TR</t>
+  </si>
+  <si>
+    <t>CI_TR</t>
+  </si>
+  <si>
+    <t>Puntaje_CS</t>
+  </si>
+  <si>
+    <t>Puntaje_CI</t>
+  </si>
+  <si>
+    <t>Género</t>
+  </si>
+  <si>
+    <t>Fecha y Hora (Entrada)</t>
+  </si>
+  <si>
+    <t>Fecha y Hora (Salida)</t>
+  </si>
+  <si>
+    <t>Total Series</t>
+  </si>
+  <si>
+    <t>Total Ensayos</t>
+  </si>
+  <si>
+    <t>Aciertos</t>
+  </si>
+  <si>
+    <t>Errores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vacios </t>
+  </si>
+  <si>
+    <t>% Acierto</t>
+  </si>
+  <si>
+    <t>Max             17</t>
+  </si>
+  <si>
+    <t>Max               30</t>
+  </si>
+  <si>
+    <t>Max                    17</t>
+  </si>
+  <si>
+    <t>Max              21</t>
+  </si>
+  <si>
+    <t>Max              18</t>
+  </si>
+  <si>
+    <t>Max                                     600.000ms</t>
+  </si>
+  <si>
+    <t>Max                                     900.000ms</t>
+  </si>
+  <si>
+    <t>Hasta que complete la tarea o tenga 2 o 3 errores</t>
+  </si>
+  <si>
+    <t>PUNTAJES BRUTOS</t>
+  </si>
+  <si>
+    <t>"[Serie 3: 524, 926, 385] [Serie 4: 2964, 6132, 4823] [Serie 5: 39871, 69748, 87924] [Serie 6: 687954, 786453, 769584] [Serie 7: 2917384, 6945817, 1562493]                    [Serie 8: 38971246, 45392168, 21458369]                                                                          [Serie 9: 398641275, 579812643, 926457183] "</t>
+  </si>
+  <si>
+    <t>"[Serie 2: 86 - P12, 52 - P10, 91 - P12] [Serie 3: 138 - P10, 214 - P8, 756 - P10] [Serie 4: 3782 - P12, 4526 - P10, 9438 - P12]                                                                         [Serie 5: 92516 - P10, 13587 - P8, 46973 - P10]                                                                    [Serie 6: 492671 - P8, 531742 - P12, 863941 - P10]                                                                                               [Serie 7: 4187529 - P8, 3975416 - P8, 9356742 - P10] "</t>
+  </si>
+  <si>
+    <t>TR no incluye el tiempo de lectura de la consigna o el tiempo de la práctica en Bloques de Corsi</t>
+  </si>
+  <si>
+    <t>TIEMPOS DE REACCIÓN</t>
+  </si>
+  <si>
+    <t>Serie_CS</t>
+  </si>
+  <si>
+    <t>Serie_CI</t>
+  </si>
+  <si>
+    <t>Hola</t>
+  </si>
+  <si>
+    <t>Total de Series Completadas en Corsi con Interferencia</t>
+  </si>
+  <si>
+    <t>POLÍGONOS - CORSI CON INTERFERENCIA</t>
+  </si>
+  <si>
+    <t>Serie Max Alcanzada en Corsi con Interferencia   [2 a 7]</t>
+  </si>
+  <si>
+    <t>Serie Max Alcanzada en Corsi Simple      [3 a 9]</t>
+  </si>
+  <si>
     <t>Tiempo Total</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t>CI</t>
-  </si>
-  <si>
-    <t>CS_TR</t>
-  </si>
-  <si>
-    <t>CI_TR</t>
-  </si>
-  <si>
-    <t>Puntaje_CS</t>
-  </si>
-  <si>
-    <t>Puntaje_CI</t>
-  </si>
-  <si>
-    <t>Género</t>
-  </si>
-  <si>
-    <t>Fecha y Hora (Entrada)</t>
-  </si>
-  <si>
-    <t>Fecha y Hora (Salida)</t>
-  </si>
-  <si>
-    <t>Total Series</t>
-  </si>
-  <si>
-    <t>Total Ensayos</t>
-  </si>
-  <si>
-    <t>Aciertos</t>
-  </si>
-  <si>
-    <t>Errores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vacios </t>
-  </si>
-  <si>
-    <t>% Acierto</t>
-  </si>
-  <si>
-    <t>Max             17</t>
-  </si>
-  <si>
-    <t>Max               30</t>
-  </si>
-  <si>
-    <t>Max                    17</t>
-  </si>
-  <si>
-    <t>Max              21</t>
-  </si>
-  <si>
-    <t>Max              18</t>
-  </si>
-  <si>
-    <t>Max                                     600.000ms</t>
-  </si>
-  <si>
-    <t>Max                                     900.000ms</t>
-  </si>
-  <si>
-    <t>Hasta que complete la tarea o tenga 2 o 3 errores</t>
-  </si>
-  <si>
-    <t>PUNTAJES BRUTOS</t>
-  </si>
-  <si>
-    <t>"[Serie 3: 524, 926, 385] [Serie 4: 2964, 6132, 4823] [Serie 5: 39871, 69748, 87924] [Serie 6: 687954, 786453, 769584] [Serie 7: 2917384, 6945817, 1562493]                    [Serie 8: 38971246, 45392168, 21458369]                                                                          [Serie 9: 398641275, 579812643, 926457183] "</t>
-  </si>
-  <si>
-    <t>"[Serie 2: 86 - P12, 52 - P10, 91 - P12] [Serie 3: 138 - P10, 214 - P8, 756 - P10] [Serie 4: 3782 - P12, 4526 - P10, 9438 - P12]                                                                         [Serie 5: 92516 - P10, 13587 - P8, 46973 - P10]                                                                    [Serie 6: 492671 - P8, 531742 - P12, 863941 - P10]                                                                                               [Serie 7: 4187529 - P8, 3975416 - P8, 9356742 - P10] "</t>
-  </si>
-  <si>
-    <t>TR no incluye el tiempo de lectura de la consigna o el tiempo de la práctica en Bloques de Corsi</t>
-  </si>
-  <si>
-    <t>TIEMPOS DE REACCIÓN</t>
-  </si>
-  <si>
-    <t>Serie_CS</t>
-  </si>
-  <si>
-    <t>Serie_CI</t>
-  </si>
-  <si>
-    <t>Hola</t>
-  </si>
-  <si>
-    <t>Total de Series Completadas en Corsi con Interferencia</t>
-  </si>
-  <si>
-    <t>POLÍGONOS - CORSI CON INTERFERENCIA</t>
-  </si>
-  <si>
-    <t>Serie Max Alcanzada en Corsi con Interferencia   [2 a 7]</t>
-  </si>
-  <si>
-    <t>Serie Max Alcanzada en Corsi Simple      [3 a 9]</t>
   </si>
 </sst>
 </file>
@@ -607,7 +607,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -672,6 +672,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -698,7 +704,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -783,19 +789,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1103,19 +1096,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1194,19 +1174,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1251,7 +1218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1274,9 +1241,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1289,16 +1253,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1310,7 +1268,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1319,37 +1277,31 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1358,31 +1310,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1391,121 +1337,118 @@
     <xf numFmtId="49" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="3" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="3" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="44" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1517,63 +1460,58 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Buena" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="369">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+  <dxfs count="368">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
+        <left/>
         <right style="thick">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1596,13 +1534,24 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="14"/>
-      </font>
-      <numFmt numFmtId="31" formatCode="[h]:mm:ss"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
-          <color theme="1"/>
+          <color indexed="64"/>
         </left>
         <right/>
         <top/>
@@ -1634,6 +1583,16 @@
         <sz val="14"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thick">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -5809,16 +5768,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <strike val="0"/>
         <outline val="0"/>
@@ -8625,8 +8574,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Estilo de tabla 1" pivot="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="368"/>
-      <tableStyleElement type="firstRowStripe" dxfId="367"/>
+      <tableStyleElement type="wholeTable" dxfId="367"/>
+      <tableStyleElement type="firstRowStripe" dxfId="366"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -8645,95 +8594,95 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:CH3" headerRowDxfId="366" dataDxfId="365" totalsRowDxfId="364">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:CH3" headerRowDxfId="365" dataDxfId="364" totalsRowDxfId="363">
   <autoFilter ref="A1:CH3"/>
   <tableColumns count="86">
-    <tableColumn id="1" name="Fecha y Hora (Entrada)" totalsRowLabel="Total" dataDxfId="363" totalsRowDxfId="362"/>
-    <tableColumn id="2" name="ID" dataDxfId="361" totalsRowDxfId="360"/>
-    <tableColumn id="3" name="Apelido" dataDxfId="359" totalsRowDxfId="358"/>
-    <tableColumn id="4" name="Nombre" dataDxfId="357" totalsRowDxfId="356"/>
-    <tableColumn id="5" name="Mail" dataDxfId="355" totalsRowDxfId="354"/>
-    <tableColumn id="6" name="Género" dataDxfId="353" totalsRowDxfId="352"/>
-    <tableColumn id="7" name="Edad" dataDxfId="351" totalsRowDxfId="350"/>
-    <tableColumn id="8" name="Carrera" dataDxfId="349" totalsRowDxfId="348"/>
-    <tableColumn id="9" name="Universidad" dataDxfId="347" totalsRowDxfId="346"/>
-    <tableColumn id="79" name="Cuatrimestre" dataDxfId="345" totalsRowDxfId="344"/>
-    <tableColumn id="78" name="Año de Ingreso" dataDxfId="343" totalsRowDxfId="342"/>
-    <tableColumn id="10" name="RA_1" dataDxfId="341" totalsRowDxfId="340"/>
-    <tableColumn id="11" name="RA_2" dataDxfId="339" totalsRowDxfId="338"/>
-    <tableColumn id="12" name="RA_3" dataDxfId="337" totalsRowDxfId="336"/>
-    <tableColumn id="13" name="RA_4" dataDxfId="335" totalsRowDxfId="334"/>
-    <tableColumn id="14" name="RA_5" dataDxfId="333" totalsRowDxfId="332"/>
-    <tableColumn id="15" name="RA_6" dataDxfId="331" totalsRowDxfId="330"/>
-    <tableColumn id="16" name="RA_7" dataDxfId="329" totalsRowDxfId="328"/>
-    <tableColumn id="17" name="RA_8" dataDxfId="327" totalsRowDxfId="326"/>
-    <tableColumn id="18" name="RA_9" dataDxfId="325" totalsRowDxfId="324"/>
-    <tableColumn id="19" name="RA_10" dataDxfId="323" totalsRowDxfId="322"/>
-    <tableColumn id="20" name="RA_11" dataDxfId="321" totalsRowDxfId="320"/>
-    <tableColumn id="21" name="RA_12" dataDxfId="319" totalsRowDxfId="318"/>
-    <tableColumn id="22" name="RA_13" dataDxfId="317" totalsRowDxfId="316"/>
-    <tableColumn id="23" name="RA_14" dataDxfId="315" totalsRowDxfId="314"/>
-    <tableColumn id="24" name="RA_15" dataDxfId="313" totalsRowDxfId="312"/>
-    <tableColumn id="25" name="RA_16" dataDxfId="311" totalsRowDxfId="310"/>
-    <tableColumn id="26" name="RA_17" dataDxfId="309" totalsRowDxfId="308"/>
-    <tableColumn id="27" name="RM_1" dataDxfId="307" totalsRowDxfId="306"/>
-    <tableColumn id="28" name="RM_2" dataDxfId="305" totalsRowDxfId="304"/>
-    <tableColumn id="29" name="RM_3" dataDxfId="303" totalsRowDxfId="302"/>
-    <tableColumn id="30" name="RM_4" dataDxfId="301" totalsRowDxfId="300"/>
-    <tableColumn id="31" name="RM_5" dataDxfId="299" totalsRowDxfId="298"/>
-    <tableColumn id="32" name="RM_6" dataDxfId="297" totalsRowDxfId="296"/>
-    <tableColumn id="33" name="RM_7" dataDxfId="295" totalsRowDxfId="294"/>
-    <tableColumn id="34" name="RM_8" dataDxfId="293" totalsRowDxfId="292"/>
-    <tableColumn id="35" name="RM_9" dataDxfId="291" totalsRowDxfId="290"/>
-    <tableColumn id="36" name="RM_10" dataDxfId="289" totalsRowDxfId="288"/>
-    <tableColumn id="37" name="RM_11" dataDxfId="287" totalsRowDxfId="286"/>
-    <tableColumn id="38" name="RM_12" dataDxfId="285" totalsRowDxfId="284"/>
-    <tableColumn id="39" name="RM_13" dataDxfId="283" totalsRowDxfId="282"/>
-    <tableColumn id="40" name="RM_14" dataDxfId="281" totalsRowDxfId="280"/>
-    <tableColumn id="41" name="RM_15" dataDxfId="279" totalsRowDxfId="278"/>
-    <tableColumn id="42" name="RM_16" dataDxfId="277" totalsRowDxfId="276"/>
-    <tableColumn id="43" name="RM_17" dataDxfId="275" totalsRowDxfId="274"/>
-    <tableColumn id="44" name="RM_18" dataDxfId="273" totalsRowDxfId="272"/>
-    <tableColumn id="45" name="RM_19" dataDxfId="271" totalsRowDxfId="270"/>
-    <tableColumn id="46" name="RM_20" dataDxfId="269" totalsRowDxfId="268"/>
-    <tableColumn id="47" name="RM_21" dataDxfId="267" totalsRowDxfId="266"/>
-    <tableColumn id="48" name="RM_22" dataDxfId="265" totalsRowDxfId="264"/>
-    <tableColumn id="49" name="RM_23" dataDxfId="263" totalsRowDxfId="262"/>
-    <tableColumn id="50" name="RM_24" dataDxfId="261" totalsRowDxfId="260"/>
-    <tableColumn id="51" name="RM_25" dataDxfId="259" totalsRowDxfId="258"/>
-    <tableColumn id="52" name="RM_26" dataDxfId="257" totalsRowDxfId="256"/>
-    <tableColumn id="53" name="RM_27" dataDxfId="255" totalsRowDxfId="254"/>
-    <tableColumn id="54" name="RM_28" dataDxfId="253" totalsRowDxfId="252"/>
-    <tableColumn id="55" name="RM_29" dataDxfId="251" totalsRowDxfId="250"/>
-    <tableColumn id="56" name="RM_30" dataDxfId="249" totalsRowDxfId="248"/>
-    <tableColumn id="57" name="RV_1" dataDxfId="247" totalsRowDxfId="246"/>
-    <tableColumn id="58" name="RV_2" dataDxfId="245" totalsRowDxfId="244"/>
-    <tableColumn id="59" name="RV_3" dataDxfId="243" totalsRowDxfId="242"/>
-    <tableColumn id="60" name="RV_4" dataDxfId="241" totalsRowDxfId="240"/>
-    <tableColumn id="61" name="RV_5" dataDxfId="239" totalsRowDxfId="238"/>
-    <tableColumn id="62" name="RV_6" dataDxfId="237" totalsRowDxfId="236"/>
-    <tableColumn id="63" name="RV_7" dataDxfId="235" totalsRowDxfId="234"/>
-    <tableColumn id="64" name="RV_8" dataDxfId="233" totalsRowDxfId="232"/>
-    <tableColumn id="65" name="RV_9" dataDxfId="231" totalsRowDxfId="230"/>
-    <tableColumn id="66" name="RV_10" dataDxfId="229" totalsRowDxfId="228"/>
-    <tableColumn id="67" name="RV_11" dataDxfId="227" totalsRowDxfId="226"/>
-    <tableColumn id="68" name="RV_12" dataDxfId="225" totalsRowDxfId="224"/>
-    <tableColumn id="69" name="RV_13" dataDxfId="223" totalsRowDxfId="222"/>
-    <tableColumn id="70" name="RV_14" dataDxfId="221" totalsRowDxfId="220"/>
-    <tableColumn id="71" name="RV_15" dataDxfId="219" totalsRowDxfId="218"/>
-    <tableColumn id="72" name="RV_16" dataDxfId="217" totalsRowDxfId="216"/>
-    <tableColumn id="73" name="RV_17" dataDxfId="215" totalsRowDxfId="214"/>
-    <tableColumn id="80" name="Respuesta_CS" dataDxfId="213" totalsRowDxfId="212"/>
-    <tableColumn id="81" name="Respuesta_CI" dataDxfId="211" totalsRowDxfId="210"/>
-    <tableColumn id="74" name="RA_TR" dataDxfId="209"/>
-    <tableColumn id="75" name="RM_TR" dataDxfId="208"/>
-    <tableColumn id="76" name="RV_TR" totalsRowFunction="count" dataDxfId="207"/>
-    <tableColumn id="84" name="CS_TR" dataDxfId="206"/>
-    <tableColumn id="83" name="CI_TR" dataDxfId="205"/>
-    <tableColumn id="85" name="Puntaje_CS" dataDxfId="204"/>
-    <tableColumn id="86" name="Puntaje_CI" dataDxfId="203"/>
-    <tableColumn id="82" name="Fecha y Hora (Salida)" dataDxfId="202"/>
-    <tableColumn id="77" name="¿Abandonó?" dataDxfId="201" totalsRowDxfId="200"/>
+    <tableColumn id="1" name="Fecha y Hora (Entrada)" totalsRowLabel="Total" dataDxfId="362" totalsRowDxfId="361"/>
+    <tableColumn id="2" name="ID" dataDxfId="360" totalsRowDxfId="359"/>
+    <tableColumn id="3" name="Apelido" dataDxfId="358" totalsRowDxfId="357"/>
+    <tableColumn id="4" name="Nombre" dataDxfId="356" totalsRowDxfId="355"/>
+    <tableColumn id="5" name="Mail" dataDxfId="354" totalsRowDxfId="353"/>
+    <tableColumn id="6" name="Género" dataDxfId="352" totalsRowDxfId="351"/>
+    <tableColumn id="7" name="Edad" dataDxfId="350" totalsRowDxfId="349"/>
+    <tableColumn id="8" name="Carrera" dataDxfId="348" totalsRowDxfId="347"/>
+    <tableColumn id="9" name="Universidad" dataDxfId="346" totalsRowDxfId="345"/>
+    <tableColumn id="79" name="Cuatrimestre" dataDxfId="344" totalsRowDxfId="343"/>
+    <tableColumn id="78" name="Año de Ingreso" dataDxfId="342" totalsRowDxfId="341"/>
+    <tableColumn id="10" name="RA_1" dataDxfId="340" totalsRowDxfId="339"/>
+    <tableColumn id="11" name="RA_2" dataDxfId="338" totalsRowDxfId="337"/>
+    <tableColumn id="12" name="RA_3" dataDxfId="336" totalsRowDxfId="335"/>
+    <tableColumn id="13" name="RA_4" dataDxfId="334" totalsRowDxfId="333"/>
+    <tableColumn id="14" name="RA_5" dataDxfId="332" totalsRowDxfId="331"/>
+    <tableColumn id="15" name="RA_6" dataDxfId="330" totalsRowDxfId="329"/>
+    <tableColumn id="16" name="RA_7" dataDxfId="328" totalsRowDxfId="327"/>
+    <tableColumn id="17" name="RA_8" dataDxfId="326" totalsRowDxfId="325"/>
+    <tableColumn id="18" name="RA_9" dataDxfId="324" totalsRowDxfId="323"/>
+    <tableColumn id="19" name="RA_10" dataDxfId="322" totalsRowDxfId="321"/>
+    <tableColumn id="20" name="RA_11" dataDxfId="320" totalsRowDxfId="319"/>
+    <tableColumn id="21" name="RA_12" dataDxfId="318" totalsRowDxfId="317"/>
+    <tableColumn id="22" name="RA_13" dataDxfId="316" totalsRowDxfId="315"/>
+    <tableColumn id="23" name="RA_14" dataDxfId="314" totalsRowDxfId="313"/>
+    <tableColumn id="24" name="RA_15" dataDxfId="312" totalsRowDxfId="311"/>
+    <tableColumn id="25" name="RA_16" dataDxfId="310" totalsRowDxfId="309"/>
+    <tableColumn id="26" name="RA_17" dataDxfId="308" totalsRowDxfId="307"/>
+    <tableColumn id="27" name="RM_1" dataDxfId="306" totalsRowDxfId="305"/>
+    <tableColumn id="28" name="RM_2" dataDxfId="304" totalsRowDxfId="303"/>
+    <tableColumn id="29" name="RM_3" dataDxfId="302" totalsRowDxfId="301"/>
+    <tableColumn id="30" name="RM_4" dataDxfId="300" totalsRowDxfId="299"/>
+    <tableColumn id="31" name="RM_5" dataDxfId="298" totalsRowDxfId="297"/>
+    <tableColumn id="32" name="RM_6" dataDxfId="296" totalsRowDxfId="295"/>
+    <tableColumn id="33" name="RM_7" dataDxfId="294" totalsRowDxfId="293"/>
+    <tableColumn id="34" name="RM_8" dataDxfId="292" totalsRowDxfId="291"/>
+    <tableColumn id="35" name="RM_9" dataDxfId="290" totalsRowDxfId="289"/>
+    <tableColumn id="36" name="RM_10" dataDxfId="288" totalsRowDxfId="287"/>
+    <tableColumn id="37" name="RM_11" dataDxfId="286" totalsRowDxfId="285"/>
+    <tableColumn id="38" name="RM_12" dataDxfId="284" totalsRowDxfId="283"/>
+    <tableColumn id="39" name="RM_13" dataDxfId="282" totalsRowDxfId="281"/>
+    <tableColumn id="40" name="RM_14" dataDxfId="280" totalsRowDxfId="279"/>
+    <tableColumn id="41" name="RM_15" dataDxfId="278" totalsRowDxfId="277"/>
+    <tableColumn id="42" name="RM_16" dataDxfId="276" totalsRowDxfId="275"/>
+    <tableColumn id="43" name="RM_17" dataDxfId="274" totalsRowDxfId="273"/>
+    <tableColumn id="44" name="RM_18" dataDxfId="272" totalsRowDxfId="271"/>
+    <tableColumn id="45" name="RM_19" dataDxfId="270" totalsRowDxfId="269"/>
+    <tableColumn id="46" name="RM_20" dataDxfId="268" totalsRowDxfId="267"/>
+    <tableColumn id="47" name="RM_21" dataDxfId="266" totalsRowDxfId="265"/>
+    <tableColumn id="48" name="RM_22" dataDxfId="264" totalsRowDxfId="263"/>
+    <tableColumn id="49" name="RM_23" dataDxfId="262" totalsRowDxfId="261"/>
+    <tableColumn id="50" name="RM_24" dataDxfId="260" totalsRowDxfId="259"/>
+    <tableColumn id="51" name="RM_25" dataDxfId="258" totalsRowDxfId="257"/>
+    <tableColumn id="52" name="RM_26" dataDxfId="256" totalsRowDxfId="255"/>
+    <tableColumn id="53" name="RM_27" dataDxfId="254" totalsRowDxfId="253"/>
+    <tableColumn id="54" name="RM_28" dataDxfId="252" totalsRowDxfId="251"/>
+    <tableColumn id="55" name="RM_29" dataDxfId="250" totalsRowDxfId="249"/>
+    <tableColumn id="56" name="RM_30" dataDxfId="248" totalsRowDxfId="247"/>
+    <tableColumn id="57" name="RV_1" dataDxfId="246" totalsRowDxfId="245"/>
+    <tableColumn id="58" name="RV_2" dataDxfId="244" totalsRowDxfId="243"/>
+    <tableColumn id="59" name="RV_3" dataDxfId="242" totalsRowDxfId="241"/>
+    <tableColumn id="60" name="RV_4" dataDxfId="240" totalsRowDxfId="239"/>
+    <tableColumn id="61" name="RV_5" dataDxfId="238" totalsRowDxfId="237"/>
+    <tableColumn id="62" name="RV_6" dataDxfId="236" totalsRowDxfId="235"/>
+    <tableColumn id="63" name="RV_7" dataDxfId="234" totalsRowDxfId="233"/>
+    <tableColumn id="64" name="RV_8" dataDxfId="232" totalsRowDxfId="231"/>
+    <tableColumn id="65" name="RV_9" dataDxfId="230" totalsRowDxfId="229"/>
+    <tableColumn id="66" name="RV_10" dataDxfId="228" totalsRowDxfId="227"/>
+    <tableColumn id="67" name="RV_11" dataDxfId="226" totalsRowDxfId="225"/>
+    <tableColumn id="68" name="RV_12" dataDxfId="224" totalsRowDxfId="223"/>
+    <tableColumn id="69" name="RV_13" dataDxfId="222" totalsRowDxfId="221"/>
+    <tableColumn id="70" name="RV_14" dataDxfId="220" totalsRowDxfId="219"/>
+    <tableColumn id="71" name="RV_15" dataDxfId="218" totalsRowDxfId="217"/>
+    <tableColumn id="72" name="RV_16" dataDxfId="216" totalsRowDxfId="215"/>
+    <tableColumn id="73" name="RV_17" dataDxfId="214" totalsRowDxfId="213"/>
+    <tableColumn id="80" name="Respuesta_CS" dataDxfId="212" totalsRowDxfId="211"/>
+    <tableColumn id="81" name="Respuesta_CI" dataDxfId="210" totalsRowDxfId="209"/>
+    <tableColumn id="74" name="RA_TR" dataDxfId="208"/>
+    <tableColumn id="75" name="RM_TR" dataDxfId="207"/>
+    <tableColumn id="76" name="RV_TR" totalsRowFunction="count" dataDxfId="206"/>
+    <tableColumn id="84" name="CS_TR" dataDxfId="205"/>
+    <tableColumn id="83" name="CI_TR" dataDxfId="204"/>
+    <tableColumn id="85" name="Puntaje_CS" dataDxfId="203"/>
+    <tableColumn id="86" name="Puntaje_CI" dataDxfId="202"/>
+    <tableColumn id="82" name="Fecha y Hora (Salida)" dataDxfId="201"/>
+    <tableColumn id="77" name="¿Abandonó?" dataDxfId="200" totalsRowDxfId="199"/>
   </tableColumns>
   <tableStyleInfo name="Estilo de tabla 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8975,10 +8924,8 @@
     <tableColumn id="85" name="RV_TR" dataDxfId="9" totalsRowDxfId="8"/>
     <tableColumn id="91" name="CS_TR" dataDxfId="7" totalsRowDxfId="6"/>
     <tableColumn id="90" name="CI_TR" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="93" name="Tiempo Total" dataDxfId="3" totalsRowDxfId="2">
-      <calculatedColumnFormula>A4-BZ4</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="80" name="¿Abandonó?" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="93" name="Tiempo Total" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="75" name="¿Abandonó?" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Estilo de tabla 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9274,10 +9221,10 @@
   <dimension ref="A1:CH86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="CF2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomRight" activeCell="CF5" sqref="CF5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -9317,262 +9264,262 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:86" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="G1" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="K1" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="L1" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD1" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF1" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG1" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH1" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI1" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ1" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="AK1" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL1" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM1" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN1" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO1" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="AP1" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ1" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="AR1" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="AS1" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="AT1" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="AU1" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="AV1" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="AW1" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX1" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY1" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="AZ1" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="BA1" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="BB1" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="BC1" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="BD1" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="BE1" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="BF1" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="BG1" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="BH1" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="BI1" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ1" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="BK1" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="BL1" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="BM1" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="BN1" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="BO1" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="BP1" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="BQ1" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="BR1" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="BS1" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="BT1" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="BU1" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="BV1" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="BW1" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="BX1" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="BY1" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="BZ1" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="CA1" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="CB1" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="CC1" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="CD1" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="CE1" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="CF1" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="CG1" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="46" t="s">
-        <v>165</v>
-      </c>
-      <c r="G1" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="45" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="45" t="s">
-        <v>153</v>
-      </c>
-      <c r="K1" s="45" t="s">
-        <v>154</v>
-      </c>
-      <c r="L1" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="45" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" s="45" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="U1" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="V1" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="W1" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="X1" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y1" s="45" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z1" s="45" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA1" s="45" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB1" s="45" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC1" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD1" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="AE1" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="AF1" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="AG1" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="AH1" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="AI1" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ1" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="AK1" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL1" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="AM1" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="AN1" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="AO1" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="AP1" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="AQ1" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR1" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AS1" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AT1" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="AU1" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="AV1" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="AW1" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="AX1" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="AY1" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="AZ1" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="BA1" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="BB1" s="45" t="s">
-        <v>49</v>
-      </c>
-      <c r="BC1" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="BD1" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="BE1" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="BF1" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="BG1" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="BH1" s="45" t="s">
-        <v>55</v>
-      </c>
-      <c r="BI1" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ1" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="BK1" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="BL1" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="BM1" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="BN1" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="BO1" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="BP1" s="45" t="s">
-        <v>63</v>
-      </c>
-      <c r="BQ1" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="BR1" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="BS1" s="45" t="s">
-        <v>66</v>
-      </c>
-      <c r="BT1" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="BU1" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="BV1" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="BW1" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="BX1" s="45" t="s">
-        <v>156</v>
-      </c>
-      <c r="BY1" s="45" t="s">
-        <v>157</v>
-      </c>
-      <c r="BZ1" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="CA1" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="CB1" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="CC1" s="45" t="s">
-        <v>161</v>
-      </c>
-      <c r="CD1" s="45" t="s">
-        <v>162</v>
-      </c>
-      <c r="CE1" s="45" t="s">
-        <v>163</v>
-      </c>
-      <c r="CF1" s="45" t="s">
-        <v>164</v>
-      </c>
-      <c r="CG1" s="45" t="s">
-        <v>167</v>
-      </c>
-      <c r="CH1" s="45" t="s">
+      <c r="CH1" s="38" t="s">
         <v>151</v>
       </c>
     </row>
@@ -9587,10 +9534,10 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -9775,10 +9722,10 @@
   <dimension ref="A1:CT9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="CK4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="CM4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="CR10" sqref="CR10"/>
+      <selection pane="bottomRight" activeCell="CS14" sqref="CS14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -9820,1468 +9767,1464 @@
     <col min="94" max="94" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="95" max="95" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="96" max="96" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="21.5703125" customWidth="1"/>
-    <col min="98" max="98" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="19.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="99" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" s="12" customFormat="1" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="21"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="26"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
-      <c r="AK1" s="25"/>
-      <c r="AL1" s="25"/>
-      <c r="AM1" s="25"/>
-      <c r="AN1" s="25"/>
-      <c r="AO1" s="25"/>
-      <c r="AP1" s="25"/>
-      <c r="AQ1" s="25"/>
-      <c r="AR1" s="25"/>
-      <c r="AS1" s="25"/>
-      <c r="AT1" s="25"/>
-      <c r="AU1" s="25"/>
-      <c r="AV1" s="25"/>
-      <c r="AW1" s="25"/>
-      <c r="AX1" s="25"/>
-      <c r="AY1" s="25"/>
-      <c r="AZ1" s="25"/>
-      <c r="BA1" s="25"/>
-      <c r="BB1" s="25"/>
-      <c r="BC1" s="25"/>
-      <c r="BD1" s="25"/>
-      <c r="BE1" s="25"/>
-      <c r="BF1" s="27"/>
-      <c r="BG1" s="26"/>
-      <c r="BH1" s="25"/>
-      <c r="BI1" s="25"/>
-      <c r="BJ1" s="25"/>
-      <c r="BK1" s="25"/>
-      <c r="BL1" s="25"/>
-      <c r="BM1" s="25"/>
-      <c r="BN1" s="25"/>
-      <c r="BO1" s="25"/>
-      <c r="BP1" s="25"/>
-      <c r="BQ1" s="25"/>
-      <c r="BR1" s="25"/>
-      <c r="BS1" s="25"/>
-      <c r="BT1" s="25"/>
-      <c r="BU1" s="25"/>
-      <c r="BV1" s="25"/>
-      <c r="BW1" s="27"/>
-      <c r="BX1" s="74" t="s">
+    <row r="1" spans="1:98" s="11" customFormat="1" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="18"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="21"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
+      <c r="Y1" s="21"/>
+      <c r="Z1" s="21"/>
+      <c r="AA1" s="21"/>
+      <c r="AB1" s="23"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="21"/>
+      <c r="AE1" s="21"/>
+      <c r="AF1" s="21"/>
+      <c r="AG1" s="21"/>
+      <c r="AH1" s="21"/>
+      <c r="AI1" s="21"/>
+      <c r="AJ1" s="21"/>
+      <c r="AK1" s="21"/>
+      <c r="AL1" s="21"/>
+      <c r="AM1" s="21"/>
+      <c r="AN1" s="21"/>
+      <c r="AO1" s="21"/>
+      <c r="AP1" s="21"/>
+      <c r="AQ1" s="21"/>
+      <c r="AR1" s="21"/>
+      <c r="AS1" s="21"/>
+      <c r="AT1" s="21"/>
+      <c r="AU1" s="21"/>
+      <c r="AV1" s="21"/>
+      <c r="AW1" s="21"/>
+      <c r="AX1" s="21"/>
+      <c r="AY1" s="21"/>
+      <c r="AZ1" s="21"/>
+      <c r="BA1" s="21"/>
+      <c r="BB1" s="21"/>
+      <c r="BC1" s="21"/>
+      <c r="BD1" s="21"/>
+      <c r="BE1" s="21"/>
+      <c r="BF1" s="23"/>
+      <c r="BG1" s="22"/>
+      <c r="BH1" s="21"/>
+      <c r="BI1" s="21"/>
+      <c r="BJ1" s="21"/>
+      <c r="BK1" s="21"/>
+      <c r="BL1" s="21"/>
+      <c r="BM1" s="21"/>
+      <c r="BN1" s="21"/>
+      <c r="BO1" s="21"/>
+      <c r="BP1" s="21"/>
+      <c r="BQ1" s="21"/>
+      <c r="BR1" s="21"/>
+      <c r="BS1" s="21"/>
+      <c r="BT1" s="21"/>
+      <c r="BU1" s="21"/>
+      <c r="BV1" s="21"/>
+      <c r="BW1" s="23"/>
+      <c r="BX1" s="69" t="s">
+        <v>182</v>
+      </c>
+      <c r="BY1" s="70" t="s">
         <v>183</v>
       </c>
-      <c r="BY1" s="75" t="s">
+      <c r="BZ1" s="17"/>
+      <c r="CA1" s="71" t="s">
+        <v>181</v>
+      </c>
+      <c r="CB1" s="72"/>
+      <c r="CC1" s="72"/>
+      <c r="CD1" s="72"/>
+      <c r="CE1" s="73"/>
+      <c r="CF1" s="73"/>
+      <c r="CG1" s="74"/>
+      <c r="CH1" s="71" t="s">
+        <v>190</v>
+      </c>
+      <c r="CI1" s="72"/>
+      <c r="CJ1" s="72"/>
+      <c r="CK1" s="72"/>
+      <c r="CL1" s="73"/>
+      <c r="CM1" s="73"/>
+      <c r="CN1" s="75" t="s">
+        <v>185</v>
+      </c>
+      <c r="CO1" s="76"/>
+      <c r="CP1" s="76"/>
+      <c r="CQ1" s="76"/>
+      <c r="CR1" s="77"/>
+      <c r="CS1" s="65" t="s">
         <v>184</v>
       </c>
-      <c r="BZ1" s="20"/>
-      <c r="CA1" s="79" t="s">
-        <v>182</v>
-      </c>
-      <c r="CB1" s="80"/>
-      <c r="CC1" s="80"/>
-      <c r="CD1" s="80"/>
-      <c r="CE1" s="81"/>
-      <c r="CF1" s="81"/>
-      <c r="CG1" s="82"/>
-      <c r="CH1" s="79" t="s">
+      <c r="CT1" s="66"/>
+    </row>
+    <row r="2" spans="1:98" s="11" customFormat="1" ht="78.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="N2" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="O2" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q2" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="S2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="T2" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="U2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="V2" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="W2" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="X2" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y2" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z2" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA2" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB2" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC2" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD2" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE2" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG2" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="AH2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="AI2" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK2" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO2" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="AP2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="AR2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="AS2" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="AT2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="AU2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="AV2" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="AW2" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="AX2" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="AY2" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="AZ2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="BA2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD2" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="BE2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="BF2" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="BG2" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="BH2" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="BI2" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="BJ2" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="BK2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="BL2" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="BM2" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="BN2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="BO2" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="BP2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="BQ2" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="BR2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="BS2" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="BT2" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="BU2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="BV2" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="BW2" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="BX2" s="69"/>
+      <c r="BY2" s="70"/>
+      <c r="BZ2" s="16"/>
+      <c r="CA2" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="CB2" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="CC2" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="CD2" s="41" t="s">
+        <v>176</v>
+      </c>
+      <c r="CE2" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="CF2" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="CG2" s="47" t="s">
         <v>191</v>
       </c>
-      <c r="CI1" s="80"/>
-      <c r="CJ1" s="80"/>
-      <c r="CK1" s="80"/>
-      <c r="CL1" s="81"/>
-      <c r="CM1" s="81"/>
-      <c r="CN1" s="83" t="s">
-        <v>186</v>
-      </c>
-      <c r="CO1" s="84"/>
-      <c r="CP1" s="84"/>
-      <c r="CQ1" s="84"/>
-      <c r="CR1" s="85"/>
-      <c r="CS1" s="76" t="s">
-        <v>185</v>
-      </c>
-      <c r="CT1" s="77"/>
-    </row>
-    <row r="2" spans="1:98" s="12" customFormat="1" ht="78.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="M2" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="N2" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="O2" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="P2" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q2" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="R2" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="S2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="T2" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="U2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="V2" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="W2" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="X2" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y2" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z2" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA2" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB2" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC2" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD2" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE2" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="AG2" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="AI2" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="AJ2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="AK2" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="AL2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="AM2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="AN2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="AO2" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="AP2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="AQ2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="AR2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="AS2" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="AT2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="AU2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="AV2" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="AW2" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="AX2" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="AY2" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="AZ2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="BA2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="BB2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="BC2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="BD2" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="BE2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="BF2" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="BG2" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="BH2" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="BI2" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="BJ2" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="BK2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="BL2" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="BM2" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="BN2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="BO2" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="BP2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="BQ2" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="BR2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="BS2" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="BT2" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="BU2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="BV2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="BW2" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="BX2" s="74"/>
-      <c r="BY2" s="75"/>
-      <c r="BZ2" s="19"/>
-      <c r="CA2" s="47" t="s">
-        <v>174</v>
-      </c>
-      <c r="CB2" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="CC2" s="48" t="s">
-        <v>176</v>
-      </c>
-      <c r="CD2" s="48" t="s">
-        <v>177</v>
-      </c>
-      <c r="CE2" s="49" t="s">
-        <v>193</v>
-      </c>
-      <c r="CF2" s="49" t="s">
+      <c r="CH2" s="61" t="s">
+        <v>189</v>
+      </c>
+      <c r="CI2" s="59"/>
+      <c r="CJ2" s="59"/>
+      <c r="CK2" s="59"/>
+      <c r="CL2" s="59"/>
+      <c r="CM2" s="60"/>
+      <c r="CN2" s="43" t="s">
         <v>178</v>
       </c>
-      <c r="CG2" s="55" t="s">
-        <v>192</v>
-      </c>
-      <c r="CH2" s="71" t="s">
-        <v>190</v>
-      </c>
-      <c r="CI2" s="69"/>
-      <c r="CJ2" s="69"/>
-      <c r="CK2" s="69"/>
-      <c r="CL2" s="69"/>
-      <c r="CM2" s="70"/>
-      <c r="CN2" s="50" t="s">
+      <c r="CO2" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="CO2" s="51" t="s">
+      <c r="CP2" s="44" t="s">
+        <v>178</v>
+      </c>
+      <c r="CQ2" s="67" t="s">
         <v>180</v>
       </c>
-      <c r="CP2" s="51" t="s">
-        <v>179</v>
-      </c>
-      <c r="CQ2" s="72" t="s">
-        <v>181</v>
-      </c>
-      <c r="CR2" s="73"/>
-      <c r="CS2" s="78"/>
-      <c r="CT2" s="77"/>
+      <c r="CR2" s="68"/>
+      <c r="CS2" s="65"/>
+      <c r="CT2" s="66"/>
     </row>
     <row r="3" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="K3" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="L3" s="81" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="P3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="R3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="S3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="T3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="U3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="V3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="W3" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="X3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA3" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB3" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC3" s="81" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD3" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF3" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG3" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH3" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ3" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="AK3" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL3" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM3" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN3" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO3" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AP3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AR3" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AS3" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AT3" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="AU3" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AV3" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AW3" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX3" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY3" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="AZ3" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="BA3" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="BB3" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="BC3" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="BD3" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="BE3" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="BF3" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="BG3" s="81" t="s">
+        <v>54</v>
+      </c>
+      <c r="BH3" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="BI3" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ3" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="BK3" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="BL3" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="BM3" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="BN3" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="BO3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="BP3" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="BQ3" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="BR3" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="BS3" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="BT3" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="BU3" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="BV3" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="BW3" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="BX3" s="81" t="s">
+        <v>156</v>
+      </c>
+      <c r="BY3" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="BZ3" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="L3" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q3" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="R3" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="S3" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="T3" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="U3" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="V3" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="W3" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="X3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y3" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z3" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB3" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC3" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD3" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="AE3" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="AF3" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="AG3" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="AH3" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AI3" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ3" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="AK3" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL3" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AM3" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="AN3" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="AO3" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="AP3" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="AQ3" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR3" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="AS3" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="AT3" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AU3" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="AV3" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="AW3" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="AX3" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="AY3" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="AZ3" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="BA3" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="BB3" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="BC3" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="BD3" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="BE3" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="BF3" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="BG3" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="BH3" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="BI3" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ3" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="BK3" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="BL3" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="BM3" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="BN3" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="BO3" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="BP3" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="BQ3" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="BR3" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="BS3" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="BT3" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="BU3" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="BV3" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="BW3" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="BX3" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="BY3" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="BZ3" s="18" t="s">
+      <c r="CA3" s="81" t="s">
+        <v>115</v>
+      </c>
+      <c r="CB3" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="CC3" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="CD3" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="CE3" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="CF3" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="CG3" s="82" t="s">
+        <v>187</v>
+      </c>
+      <c r="CH3" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="CA3" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="CB3" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="CC3" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="CD3" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="CE3" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="CF3" s="13" t="s">
+      <c r="CI3" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="CJ3" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="CK3" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="CL3" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="CM3" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="CN3" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="CO3" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="CP3" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="CQ3" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="CG3" s="56" t="s">
-        <v>188</v>
-      </c>
-      <c r="CH3" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="CI3" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="CJ3" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="CK3" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="CL3" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="CM3" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="CN3" s="57" t="s">
-        <v>71</v>
-      </c>
-      <c r="CO3" s="58" t="s">
-        <v>72</v>
-      </c>
-      <c r="CP3" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="CQ3" s="18" t="s">
+      <c r="CR3" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="CR3" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="CS3" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="CT3" s="22" t="s">
+      <c r="CS3" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="CT3" s="19" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:98" x14ac:dyDescent="0.3">
-      <c r="A4" s="59"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="62">
+      <c r="A4" s="50"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="53">
         <f>IF(Original!L2 = Corrección!$L$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="M4" s="60">
+      <c r="M4" s="51">
         <f>IF(Original!M2 = Corrección!$M$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="N4" s="60">
+      <c r="N4" s="51">
         <f>IF(Original!N2 = Corrección!$N$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="O4" s="60">
+      <c r="O4" s="51">
         <f>IF(Original!O2 = Corrección!$O$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="P4" s="60">
+      <c r="P4" s="51">
         <f>IF(Original!P2 = Corrección!$P$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="60">
+      <c r="Q4" s="51">
         <f>IF(Original!Q2 = Corrección!$Q$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="R4" s="60">
+      <c r="R4" s="51">
         <f>IF(Original!R2 = Corrección!$R$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="S4" s="60">
+      <c r="S4" s="51">
         <f>IF(Original!S2 = Corrección!$S$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="T4" s="60">
+      <c r="T4" s="51">
         <f>IF(Original!T2 = Corrección!$T$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="U4" s="60">
+      <c r="U4" s="51">
         <f>IF(Original!U2 = Corrección!$U$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="V4" s="60">
+      <c r="V4" s="51">
         <f>IF(Original!V2 = Corrección!$V$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="W4" s="60">
+      <c r="W4" s="51">
         <f>IF(Original!W2 = Corrección!$W$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="X4" s="60">
+      <c r="X4" s="51">
         <f>IF(Original!X2 = Corrección!$X$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Y4" s="60">
+      <c r="Y4" s="51">
         <f>IF(Original!Y2 = Corrección!$Y$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Z4" s="60">
+      <c r="Z4" s="51">
         <f>IF(Original!Z2 = Corrección!$Z$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AA4" s="60">
+      <c r="AA4" s="51">
         <f>IF(Original!AA2 = Corrección!$AA$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AB4" s="63">
+      <c r="AB4" s="54">
         <f>IF(Original!AB2 = Corrección!$AB$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AC4" s="62">
+      <c r="AC4" s="53">
         <f>IF(Original!AC2 = Corrección!$AC$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AD4" s="60">
+      <c r="AD4" s="51">
         <f>IF(Original!AD2 = Corrección!$AD$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AE4" s="60">
+      <c r="AE4" s="51">
         <f>IF(Original!AE2 = Corrección!$AE$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AF4" s="60">
+      <c r="AF4" s="51">
         <f>IF(Original!AF2 = Corrección!$AF$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AG4" s="60">
+      <c r="AG4" s="51">
         <f>IF(Original!AG2 = Corrección!$AG$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AH4" s="60">
+      <c r="AH4" s="51">
         <f>IF(Original!AH2 = Corrección!$AH$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AI4" s="60">
+      <c r="AI4" s="51">
         <f>IF(Original!AI2 = Corrección!$AI$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AJ4" s="60">
+      <c r="AJ4" s="51">
         <f>IF(Original!AJ2 = Corrección!$AJ$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AK4" s="60">
+      <c r="AK4" s="51">
         <f>IF(Original!AK2 = Corrección!$AK$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AL4" s="60">
+      <c r="AL4" s="51">
         <f>IF(Original!AL2 = Corrección!$AL$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AM4" s="60">
+      <c r="AM4" s="51">
         <f>IF(Original!AM2 = Corrección!$AM$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AN4" s="60">
+      <c r="AN4" s="51">
         <f>IF(Original!AN2 = Corrección!$AN$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AO4" s="60">
+      <c r="AO4" s="51">
         <f>IF(Original!AO2 = Corrección!$AO$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AP4" s="60">
+      <c r="AP4" s="51">
         <f>IF(Original!AP2 = Corrección!$AP$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AQ4" s="60">
+      <c r="AQ4" s="51">
         <f>IF(Original!AQ2 = Corrección!$AQ$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AR4" s="60">
+      <c r="AR4" s="51">
         <f>IF(Original!AR2 = Corrección!$AR$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AS4" s="60">
+      <c r="AS4" s="51">
         <f>IF(Original!AS2 = Corrección!$AS$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AT4" s="60">
+      <c r="AT4" s="51">
         <f>IF(Original!AT2 = Corrección!$AT$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AU4" s="60">
+      <c r="AU4" s="51">
         <f>IF(Original!AU2 = Corrección!$AU$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AV4" s="60">
+      <c r="AV4" s="51">
         <f>IF(Original!AV2 = Corrección!$AV$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AW4" s="60">
+      <c r="AW4" s="51">
         <f>IF(Original!AW2 = Corrección!$AW$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AX4" s="60">
+      <c r="AX4" s="51">
         <f>IF(Original!AX2 = Corrección!$AX$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AY4" s="60">
+      <c r="AY4" s="51">
         <f>IF(Original!AY2 = Corrección!$AY$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AZ4" s="60">
+      <c r="AZ4" s="51">
         <f>IF(Original!AZ2 = Corrección!$AZ$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BA4" s="60">
+      <c r="BA4" s="51">
         <f>IF(Original!BA2 = Corrección!$BA$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BB4" s="60">
+      <c r="BB4" s="51">
         <f>IF(Original!BB2 = Corrección!$BB$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BC4" s="60">
+      <c r="BC4" s="51">
         <f>IF(Original!BC2 = Corrección!$BC$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BD4" s="60">
+      <c r="BD4" s="51">
         <f>IF(Original!BD2 = Corrección!$BD$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BE4" s="60">
+      <c r="BE4" s="51">
         <f>IF(Original!BE2 = Corrección!$BE$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BF4" s="63">
+      <c r="BF4" s="54">
         <f>IF(Original!BF2 = Corrección!$BF$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BG4" s="62">
+      <c r="BG4" s="53">
         <f>IF(Original!BG2 = Corrección!$BG$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BH4" s="60">
+      <c r="BH4" s="51">
         <f>IF(Original!BH2 = Corrección!$BH$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BI4" s="60">
+      <c r="BI4" s="51">
         <f>IF(Original!BI2 = Corrección!$BI$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BJ4" s="60">
+      <c r="BJ4" s="51">
         <f>IF(Original!BJ2 = Corrección!$BJ$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BK4" s="60">
+      <c r="BK4" s="51">
         <f>IF(Original!BK2 = Corrección!$BK$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BL4" s="60">
+      <c r="BL4" s="51">
         <f>IF(Original!BL2 = Corrección!$BL$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BM4" s="60">
+      <c r="BM4" s="51">
         <f>IF(Original!BM2 = Corrección!$BM$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BN4" s="60">
+      <c r="BN4" s="51">
         <f>IF(Original!BN2 = Corrección!$BN$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BO4" s="60">
+      <c r="BO4" s="51">
         <f>IF(Original!BO2 = Corrección!$BO$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BP4" s="60">
+      <c r="BP4" s="51">
         <f>IF(Original!BP2 = Corrección!$BP$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BQ4" s="60">
+      <c r="BQ4" s="51">
         <f>IF(Original!BQ2 = Corrección!$BQ$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BR4" s="60">
+      <c r="BR4" s="51">
         <f>IF(Original!BR2 = Corrección!$BR$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BS4" s="60">
+      <c r="BS4" s="51">
         <f>IF(Original!BS2 = Corrección!$BS$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BT4" s="60">
+      <c r="BT4" s="51">
         <f>IF(Original!BT2 = Corrección!$BT$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BU4" s="60">
+      <c r="BU4" s="51">
         <f>IF(Original!BU2 = Corrección!$BU$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BV4" s="60">
+      <c r="BV4" s="51">
         <f>IF(Original!BV2 = Corrección!$BV$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BW4" s="63">
+      <c r="BW4" s="54">
         <f>IF(Original!BW2 = Corrección!$BW$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BX4" s="62"/>
-      <c r="BY4" s="63"/>
-      <c r="BZ4" s="64"/>
-      <c r="CA4" s="62">
+      <c r="BX4" s="53"/>
+      <c r="BY4" s="54"/>
+      <c r="BZ4" s="55"/>
+      <c r="CA4" s="53">
         <f t="shared" ref="CA4" si="0">SUM(L4:AB4)</f>
         <v>0</v>
       </c>
-      <c r="CB4" s="60">
+      <c r="CB4" s="51">
         <f t="shared" ref="CB4" si="1">SUM(AC4:BF4)</f>
         <v>0</v>
       </c>
-      <c r="CC4" s="60">
+      <c r="CC4" s="51">
         <f t="shared" ref="CC4:CC5" si="2">SUM(BG4:BW4)</f>
         <v>0</v>
       </c>
-      <c r="CD4" s="60"/>
-      <c r="CE4" s="60"/>
-      <c r="CF4" s="60"/>
-      <c r="CG4" s="65"/>
-      <c r="CH4" s="60">
+      <c r="CD4" s="51"/>
+      <c r="CE4" s="51"/>
+      <c r="CF4" s="51"/>
+      <c r="CG4" s="56"/>
+      <c r="CH4" s="51">
         <v>1</v>
       </c>
-      <c r="CI4" s="60">
+      <c r="CI4" s="51">
         <f>CH4*3</f>
         <v>3</v>
       </c>
-      <c r="CJ4" s="60">
-        <v>0</v>
-      </c>
-      <c r="CK4" s="60"/>
-      <c r="CL4" s="60"/>
-      <c r="CM4" s="66">
+      <c r="CJ4" s="51">
+        <v>0</v>
+      </c>
+      <c r="CK4" s="51"/>
+      <c r="CL4" s="51"/>
+      <c r="CM4" s="57">
         <f t="shared" ref="CM4:CM5" si="3">(CJ4/CI4)*100</f>
         <v>0</v>
       </c>
-      <c r="CN4" s="67"/>
-      <c r="CO4" s="60"/>
-      <c r="CP4" s="60"/>
-      <c r="CQ4" s="60"/>
-      <c r="CR4" s="60"/>
-      <c r="CS4" s="68">
-        <f t="shared" ref="CS4:CS5" si="4">A4-BZ4</f>
-        <v>0</v>
-      </c>
+      <c r="CN4" s="58">
+        <v>100</v>
+      </c>
+      <c r="CO4" s="51"/>
+      <c r="CP4" s="51"/>
+      <c r="CQ4" s="51"/>
+      <c r="CR4" s="54"/>
+      <c r="CS4" s="53"/>
       <c r="CT4" s="63"/>
     </row>
     <row r="5" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
-      <c r="L5" s="34">
+      <c r="L5" s="28">
         <f>IF(Original!L3 = Corrección!$L$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="M5" s="35">
+      <c r="M5" s="29">
         <f>IF(Original!M3 = Corrección!$M$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="N5" s="35">
+      <c r="N5" s="29">
         <f>IF(Original!N3 = Corrección!$N$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="O5" s="35">
+      <c r="O5" s="29">
         <f>IF(Original!O3 = Corrección!$O$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="P5" s="35">
+      <c r="P5" s="29">
         <f>IF(Original!P3 = Corrección!$P$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="35">
+      <c r="Q5" s="29">
         <f>IF(Original!Q3 = Corrección!$Q$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="R5" s="35">
+      <c r="R5" s="29">
         <f>IF(Original!R3 = Corrección!$R$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="S5" s="35">
+      <c r="S5" s="29">
         <f>IF(Original!S3 = Corrección!$S$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="T5" s="35">
+      <c r="T5" s="29">
         <f>IF(Original!T3 = Corrección!$T$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="U5" s="35">
+      <c r="U5" s="29">
         <f>IF(Original!U3 = Corrección!$U$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="V5" s="35">
+      <c r="V5" s="29">
         <f>IF(Original!V3 = Corrección!$V$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="W5" s="35">
+      <c r="W5" s="29">
         <f>IF(Original!W3 = Corrección!$W$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="X5" s="35">
+      <c r="X5" s="29">
         <f>IF(Original!X3 = Corrección!$X$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Y5" s="35">
+      <c r="Y5" s="29">
         <f>IF(Original!Y3 = Corrección!$Y$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Z5" s="35">
+      <c r="Z5" s="29">
         <f>IF(Original!Z3 = Corrección!$Z$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AA5" s="35">
+      <c r="AA5" s="29">
         <f>IF(Original!AA3 = Corrección!$AA$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AB5" s="36">
+      <c r="AB5" s="30">
         <f>IF(Original!AB3 = Corrección!$AB$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AC5" s="34">
+      <c r="AC5" s="28">
         <f>IF(Original!AC3 = Corrección!$AC$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AD5" s="35">
+      <c r="AD5" s="29">
         <f>IF(Original!AD3 = Corrección!$AD$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AE5" s="35">
+      <c r="AE5" s="29">
         <f>IF(Original!AE3 = Corrección!$AE$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AF5" s="35">
+      <c r="AF5" s="29">
         <f>IF(Original!AF3 = Corrección!$AF$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AG5" s="35">
+      <c r="AG5" s="29">
         <f>IF(Original!AG3 = Corrección!$AG$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AH5" s="35">
+      <c r="AH5" s="29">
         <f>IF(Original!AH3 = Corrección!$AH$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AI5" s="35">
+      <c r="AI5" s="29">
         <f>IF(Original!AI3 = Corrección!$AI$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AJ5" s="35">
+      <c r="AJ5" s="29">
         <f>IF(Original!AJ3 = Corrección!$AJ$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AK5" s="35">
+      <c r="AK5" s="29">
         <f>IF(Original!AK3 = Corrección!$AK$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AL5" s="35">
+      <c r="AL5" s="29">
         <f>IF(Original!AL3 = Corrección!$AL$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AM5" s="35">
+      <c r="AM5" s="29">
         <f>IF(Original!AM3 = Corrección!$AM$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AN5" s="37">
+      <c r="AN5" s="31">
         <f>IF(Original!AN3 = Corrección!$AN$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AO5" s="37">
+      <c r="AO5" s="31">
         <f>IF(Original!AO3 = Corrección!$AO$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AP5" s="37">
+      <c r="AP5" s="31">
         <f>IF(Original!AP3 = Corrección!$AP$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AQ5" s="37">
+      <c r="AQ5" s="31">
         <f>IF(Original!AQ3 = Corrección!$AQ$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AR5" s="37">
+      <c r="AR5" s="31">
         <f>IF(Original!AR3 = Corrección!$AR$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AS5" s="37">
+      <c r="AS5" s="31">
         <f>IF(Original!AS3 = Corrección!$AS$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AT5" s="37">
+      <c r="AT5" s="31">
         <f>IF(Original!AT3 = Corrección!$AT$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AU5" s="37">
+      <c r="AU5" s="31">
         <f>IF(Original!AU3 = Corrección!$AU$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AV5" s="37">
+      <c r="AV5" s="31">
         <f>IF(Original!AV3 = Corrección!$AV$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AW5" s="37">
+      <c r="AW5" s="31">
         <f>IF(Original!AW3 = Corrección!$AW$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AX5" s="37">
+      <c r="AX5" s="31">
         <f>IF(Original!AX3 = Corrección!$AX$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AY5" s="37">
+      <c r="AY5" s="31">
         <f>IF(Original!AY3 = Corrección!$AY$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="AZ5" s="37">
+      <c r="AZ5" s="31">
         <f>IF(Original!AZ3 = Corrección!$AZ$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BA5" s="37">
+      <c r="BA5" s="31">
         <f>IF(Original!BA3 = Corrección!$BA$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BB5" s="37">
+      <c r="BB5" s="31">
         <f>IF(Original!BB3 = Corrección!$BB$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BC5" s="37">
+      <c r="BC5" s="31">
         <f>IF(Original!BC3 = Corrección!$BC$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BD5" s="37">
+      <c r="BD5" s="31">
         <f>IF(Original!BD3 = Corrección!$BD$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BE5" s="37">
+      <c r="BE5" s="31">
         <f>IF(Original!BE3 = Corrección!$BE$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BF5" s="38">
+      <c r="BF5" s="32">
         <f>IF(Original!BF3 = Corrección!$BF$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BG5" s="39">
+      <c r="BG5" s="33">
         <f>IF(Original!BG3 = Corrección!$BG$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BH5" s="37">
+      <c r="BH5" s="31">
         <f>IF(Original!BH3 = Corrección!$BH$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BI5" s="37">
+      <c r="BI5" s="31">
         <f>IF(Original!BI3 = Corrección!$BI$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BJ5" s="37">
+      <c r="BJ5" s="31">
         <f>IF(Original!BJ3 = Corrección!$BJ$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BK5" s="37">
+      <c r="BK5" s="31">
         <f>IF(Original!BK3 = Corrección!$BK$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BL5" s="37">
+      <c r="BL5" s="31">
         <f>IF(Original!BL3 = Corrección!$BL$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BM5" s="37">
+      <c r="BM5" s="31">
         <f>IF(Original!BM3 = Corrección!$BM$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BN5" s="37">
+      <c r="BN5" s="31">
         <f>IF(Original!BN3 = Corrección!$BN$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BO5" s="37">
+      <c r="BO5" s="31">
         <f>IF(Original!BO3 = Corrección!$BO$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BP5" s="37">
+      <c r="BP5" s="31">
         <f>IF(Original!BP3 = Corrección!$BP$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BQ5" s="37">
+      <c r="BQ5" s="31">
         <f>IF(Original!BQ3 = Corrección!$BQ$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BR5" s="37">
+      <c r="BR5" s="31">
         <f>IF(Original!BR3 = Corrección!$BR$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BS5" s="37">
+      <c r="BS5" s="31">
         <f>IF(Original!BS3 = Corrección!$BS$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BT5" s="37">
+      <c r="BT5" s="31">
         <f>IF(Original!BT3 = Corrección!$BT$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BU5" s="37">
+      <c r="BU5" s="31">
         <f>IF(Original!BU3 = Corrección!$BU$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BV5" s="37">
+      <c r="BV5" s="31">
         <f>IF(Original!BV3 = Corrección!$BV$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BW5" s="38">
+      <c r="BW5" s="32">
         <f>IF(Original!BW3 = Corrección!$BW$2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="BX5" s="40"/>
-      <c r="BY5" s="41"/>
-      <c r="BZ5" s="53"/>
-      <c r="CA5" s="42">
+      <c r="BX5" s="34"/>
+      <c r="BY5" s="35"/>
+      <c r="BZ5" s="46"/>
+      <c r="CA5" s="36">
         <f>SUM(L5:AB5)</f>
         <v>0</v>
       </c>
-      <c r="CB5" s="15">
-        <f t="shared" ref="CB5" si="5">SUM(BF5:BV5)</f>
-        <v>0</v>
-      </c>
-      <c r="CC5" s="15">
+      <c r="CB5" s="13">
+        <f t="shared" ref="CB5" si="4">SUM(BF5:BV5)</f>
+        <v>0</v>
+      </c>
+      <c r="CC5" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="CD5" s="15"/>
-      <c r="CE5" s="15"/>
-      <c r="CF5" s="15"/>
-      <c r="CG5" s="36"/>
-      <c r="CH5" s="15">
+      <c r="CD5" s="13"/>
+      <c r="CE5" s="13"/>
+      <c r="CF5" s="13"/>
+      <c r="CG5" s="30"/>
+      <c r="CH5" s="13">
         <v>1</v>
       </c>
-      <c r="CI5" s="15">
+      <c r="CI5" s="13">
         <f>CH5*3</f>
         <v>3</v>
       </c>
-      <c r="CJ5" s="15">
-        <v>0</v>
-      </c>
-      <c r="CK5" s="15"/>
-      <c r="CL5" s="15"/>
-      <c r="CM5" s="52">
+      <c r="CJ5" s="13">
+        <v>0</v>
+      </c>
+      <c r="CK5" s="13"/>
+      <c r="CL5" s="13"/>
+      <c r="CM5" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="CN5" s="44"/>
-      <c r="CO5" s="15"/>
-      <c r="CP5" s="15"/>
-      <c r="CQ5" s="15"/>
-      <c r="CR5" s="15"/>
-      <c r="CS5" s="54">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="CT5" s="43"/>
+      <c r="CN5" s="37">
+        <v>100</v>
+      </c>
+      <c r="CO5" s="13"/>
+      <c r="CP5" s="13"/>
+      <c r="CQ5" s="13"/>
+      <c r="CR5" s="62"/>
+      <c r="CS5" s="64"/>
+      <c r="CT5" s="63"/>
     </row>
     <row r="6" spans="1:98" x14ac:dyDescent="0.3">
       <c r="F6" s="4"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="15"/>
-      <c r="AA6" s="15"/>
-      <c r="AB6" s="15"/>
-      <c r="AC6" s="15"/>
-      <c r="AD6" s="15"/>
-      <c r="AE6" s="15"/>
-      <c r="AF6" s="15"/>
-      <c r="AG6" s="15"/>
-      <c r="AH6" s="15"/>
-      <c r="AI6" s="15"/>
-      <c r="AJ6" s="15"/>
-      <c r="AK6" s="15"/>
-      <c r="AL6" s="15"/>
-      <c r="AM6" s="15"/>
-      <c r="AN6" s="15"/>
-      <c r="AO6" s="15"/>
-      <c r="AP6" s="15"/>
-      <c r="AQ6" s="15"/>
-      <c r="AR6" s="15"/>
-      <c r="AS6" s="15"/>
-      <c r="AT6" s="15"/>
-      <c r="AU6" s="15"/>
-      <c r="AV6" s="15"/>
-      <c r="AW6" s="15"/>
-      <c r="AX6" s="15"/>
-      <c r="AY6" s="15"/>
-      <c r="AZ6" s="15"/>
-      <c r="BA6" s="15"/>
-      <c r="BB6" s="15"/>
-      <c r="BC6" s="15"/>
-      <c r="BD6" s="15"/>
-      <c r="BE6" s="15"/>
-      <c r="BF6" s="15"/>
-      <c r="BG6" s="15"/>
-      <c r="BH6" s="15"/>
-      <c r="BI6" s="15"/>
-      <c r="BJ6" s="15"/>
-      <c r="BK6" s="15"/>
-      <c r="BL6" s="15"/>
-      <c r="BM6" s="15"/>
-      <c r="BN6" s="15"/>
-      <c r="BO6" s="15"/>
-      <c r="BP6" s="15"/>
-      <c r="BQ6" s="15"/>
-      <c r="BR6" s="15"/>
-      <c r="BS6" s="15"/>
-      <c r="BT6" s="15"/>
-      <c r="BU6" s="15"/>
-      <c r="BV6" s="15"/>
-      <c r="BW6" s="15"/>
-      <c r="BX6" s="15"/>
-      <c r="BY6" s="15"/>
-      <c r="BZ6" s="14"/>
-      <c r="CA6" s="15"/>
-      <c r="CB6" s="15"/>
-      <c r="CC6" s="15"/>
-      <c r="CD6" s="15"/>
-      <c r="CE6" s="15"/>
-      <c r="CF6" s="15"/>
-      <c r="CG6" s="15"/>
-      <c r="CH6" s="15"/>
-      <c r="CI6" s="15"/>
-      <c r="CJ6" s="15"/>
-      <c r="CK6" s="15"/>
-      <c r="CL6" s="15"/>
-      <c r="CM6" s="15"/>
-      <c r="CN6" s="14"/>
-      <c r="CO6" s="14"/>
-      <c r="CP6" s="14"/>
-      <c r="CQ6" s="14"/>
-      <c r="CR6" s="14"/>
-      <c r="CS6" s="14"/>
-      <c r="CT6" s="33"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13"/>
+      <c r="W6" s="13"/>
+      <c r="X6" s="13"/>
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="13"/>
+      <c r="AA6" s="13"/>
+      <c r="AB6" s="13"/>
+      <c r="AC6" s="13"/>
+      <c r="AD6" s="13"/>
+      <c r="AE6" s="13"/>
+      <c r="AF6" s="13"/>
+      <c r="AG6" s="13"/>
+      <c r="AH6" s="13"/>
+      <c r="AI6" s="13"/>
+      <c r="AJ6" s="13"/>
+      <c r="AK6" s="13"/>
+      <c r="AL6" s="13"/>
+      <c r="AM6" s="13"/>
+      <c r="AN6" s="13"/>
+      <c r="AO6" s="13"/>
+      <c r="AP6" s="13"/>
+      <c r="AQ6" s="13"/>
+      <c r="AR6" s="13"/>
+      <c r="AS6" s="13"/>
+      <c r="AT6" s="13"/>
+      <c r="AU6" s="13"/>
+      <c r="AV6" s="13"/>
+      <c r="AW6" s="13"/>
+      <c r="AX6" s="13"/>
+      <c r="AY6" s="13"/>
+      <c r="AZ6" s="13"/>
+      <c r="BA6" s="13"/>
+      <c r="BB6" s="13"/>
+      <c r="BC6" s="13"/>
+      <c r="BD6" s="13"/>
+      <c r="BE6" s="13"/>
+      <c r="BF6" s="13"/>
+      <c r="BG6" s="13"/>
+      <c r="BH6" s="13"/>
+      <c r="BI6" s="13"/>
+      <c r="BJ6" s="13"/>
+      <c r="BK6" s="13"/>
+      <c r="BL6" s="13"/>
+      <c r="BM6" s="13"/>
+      <c r="BN6" s="13"/>
+      <c r="BO6" s="13"/>
+      <c r="BP6" s="13"/>
+      <c r="BQ6" s="13"/>
+      <c r="BR6" s="13"/>
+      <c r="BS6" s="13"/>
+      <c r="BT6" s="13"/>
+      <c r="BU6" s="13"/>
+      <c r="BV6" s="13"/>
+      <c r="BW6" s="13"/>
+      <c r="BX6" s="13"/>
+      <c r="BY6" s="13"/>
+      <c r="BZ6" s="12"/>
+      <c r="CA6" s="13"/>
+      <c r="CB6" s="13"/>
+      <c r="CC6" s="13"/>
+      <c r="CD6" s="13"/>
+      <c r="CE6" s="13"/>
+      <c r="CF6" s="13"/>
+      <c r="CG6" s="13"/>
+      <c r="CH6" s="13"/>
+      <c r="CI6" s="13"/>
+      <c r="CJ6" s="13"/>
+      <c r="CK6" s="13"/>
+      <c r="CL6" s="13"/>
+      <c r="CM6" s="13"/>
+      <c r="CN6" s="12"/>
+      <c r="CO6" s="12"/>
+      <c r="CP6" s="12"/>
+      <c r="CQ6" s="12"/>
+      <c r="CR6" s="12"/>
+      <c r="CS6" s="12"/>
     </row>
     <row r="7" spans="1:98" x14ac:dyDescent="0.3">
       <c r="F7" s="4"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
-      <c r="T7" s="15"/>
-      <c r="U7" s="15"/>
-      <c r="V7" s="15"/>
-      <c r="W7" s="15"/>
-      <c r="X7" s="15"/>
-      <c r="Y7" s="15"/>
-      <c r="Z7" s="15"/>
-      <c r="AA7" s="15"/>
-      <c r="AB7" s="15"/>
-      <c r="AC7" s="15"/>
-      <c r="AD7" s="15"/>
-      <c r="AE7" s="15"/>
-      <c r="AF7" s="15"/>
-      <c r="AG7" s="15"/>
-      <c r="AH7" s="15"/>
-      <c r="AI7" s="15"/>
-      <c r="AJ7" s="15"/>
-      <c r="AK7" s="15"/>
-      <c r="AL7" s="15"/>
-      <c r="AM7" s="15"/>
-      <c r="AN7" s="15"/>
-      <c r="AO7" s="15"/>
-      <c r="AP7" s="15"/>
-      <c r="AQ7" s="15"/>
-      <c r="AR7" s="15"/>
-      <c r="AS7" s="15"/>
-      <c r="AT7" s="15"/>
-      <c r="AU7" s="15"/>
-      <c r="AV7" s="15"/>
-      <c r="AW7" s="15"/>
-      <c r="AX7" s="15"/>
-      <c r="AY7" s="15"/>
-      <c r="AZ7" s="15"/>
-      <c r="BA7" s="15"/>
-      <c r="BB7" s="15"/>
-      <c r="BC7" s="15"/>
-      <c r="BD7" s="15"/>
-      <c r="BE7" s="15"/>
-      <c r="BF7" s="15"/>
-      <c r="BG7" s="15"/>
-      <c r="BH7" s="15"/>
-      <c r="BI7" s="15"/>
-      <c r="BJ7" s="15"/>
-      <c r="BK7" s="15"/>
-      <c r="BL7" s="15"/>
-      <c r="BM7" s="15"/>
-      <c r="BN7" s="15"/>
-      <c r="BO7" s="15"/>
-      <c r="BP7" s="15"/>
-      <c r="BQ7" s="15"/>
-      <c r="BR7" s="15"/>
-      <c r="BS7" s="15"/>
-      <c r="BT7" s="15"/>
-      <c r="BU7" s="15"/>
-      <c r="BV7" s="15"/>
-      <c r="BW7" s="15"/>
-      <c r="BX7" s="15"/>
-      <c r="BY7" s="15"/>
-      <c r="BZ7" s="14"/>
-      <c r="CA7" s="15"/>
-      <c r="CB7" s="15"/>
-      <c r="CC7" s="15"/>
-      <c r="CD7" s="15"/>
-      <c r="CE7" s="15"/>
-      <c r="CF7" s="15"/>
-      <c r="CG7" s="15"/>
-      <c r="CH7" s="15"/>
-      <c r="CI7" s="15"/>
-      <c r="CJ7" s="15"/>
-      <c r="CK7" s="15"/>
-      <c r="CL7" s="15"/>
-      <c r="CM7" s="15"/>
-      <c r="CN7" s="14"/>
-      <c r="CO7" s="14"/>
-      <c r="CP7" s="14"/>
-      <c r="CQ7" s="14"/>
-      <c r="CR7" s="14"/>
-      <c r="CS7" s="14"/>
-      <c r="CT7" s="33"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="13"/>
+      <c r="X7" s="13"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="13"/>
+      <c r="AA7" s="13"/>
+      <c r="AB7" s="13"/>
+      <c r="AC7" s="13"/>
+      <c r="AD7" s="13"/>
+      <c r="AE7" s="13"/>
+      <c r="AF7" s="13"/>
+      <c r="AG7" s="13"/>
+      <c r="AH7" s="13"/>
+      <c r="AI7" s="13"/>
+      <c r="AJ7" s="13"/>
+      <c r="AK7" s="13"/>
+      <c r="AL7" s="13"/>
+      <c r="AM7" s="13"/>
+      <c r="AN7" s="13"/>
+      <c r="AO7" s="13"/>
+      <c r="AP7" s="13"/>
+      <c r="AQ7" s="13"/>
+      <c r="AR7" s="13"/>
+      <c r="AS7" s="13"/>
+      <c r="AT7" s="13"/>
+      <c r="AU7" s="13"/>
+      <c r="AV7" s="13"/>
+      <c r="AW7" s="13"/>
+      <c r="AX7" s="13"/>
+      <c r="AY7" s="13"/>
+      <c r="AZ7" s="13"/>
+      <c r="BA7" s="13"/>
+      <c r="BB7" s="13"/>
+      <c r="BC7" s="13"/>
+      <c r="BD7" s="13"/>
+      <c r="BE7" s="13"/>
+      <c r="BF7" s="13"/>
+      <c r="BG7" s="13"/>
+      <c r="BH7" s="13"/>
+      <c r="BI7" s="13"/>
+      <c r="BJ7" s="13"/>
+      <c r="BK7" s="13"/>
+      <c r="BL7" s="13"/>
+      <c r="BM7" s="13"/>
+      <c r="BN7" s="13"/>
+      <c r="BO7" s="13"/>
+      <c r="BP7" s="13"/>
+      <c r="BQ7" s="13"/>
+      <c r="BR7" s="13"/>
+      <c r="BS7" s="13"/>
+      <c r="BT7" s="13"/>
+      <c r="BU7" s="13"/>
+      <c r="BV7" s="13"/>
+      <c r="BW7" s="13"/>
+      <c r="BX7" s="13"/>
+      <c r="BY7" s="13"/>
+      <c r="BZ7" s="12"/>
+      <c r="CA7" s="13"/>
+      <c r="CB7" s="13"/>
+      <c r="CC7" s="13"/>
+      <c r="CD7" s="13"/>
+      <c r="CE7" s="13"/>
+      <c r="CF7" s="13"/>
+      <c r="CG7" s="13"/>
+      <c r="CH7" s="13"/>
+      <c r="CI7" s="13"/>
+      <c r="CJ7" s="13"/>
+      <c r="CK7" s="13"/>
+      <c r="CL7" s="13"/>
+      <c r="CM7" s="13"/>
+      <c r="CN7" s="12"/>
+      <c r="CO7" s="12"/>
+      <c r="CP7" s="12"/>
+      <c r="CQ7" s="12"/>
+      <c r="CR7" s="12"/>
+      <c r="CS7" s="12"/>
     </row>
     <row r="8" spans="1:98" x14ac:dyDescent="0.3">
       <c r="F8" s="4"/>
@@ -11301,19 +11244,14 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="CS1:CT2"/>
     <mergeCell ref="CQ2:CR2"/>
     <mergeCell ref="BX1:BX2"/>
     <mergeCell ref="BY1:BY2"/>
-    <mergeCell ref="CS1:CT2"/>
     <mergeCell ref="CA1:CG1"/>
     <mergeCell ref="CN1:CR1"/>
     <mergeCell ref="CH1:CM1"/>
   </mergeCells>
-  <conditionalFormatting sqref="CT4:CT7">
-    <cfRule type="containsText" dxfId="199" priority="1" operator="containsText" text="R">
-      <formula>NOT(ISERROR(SEARCH("R",CT4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
@@ -11462,12 +11400,12 @@
       </c>
     </row>
     <row r="3" spans="2:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="78" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="88"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="80"/>
       <c r="I3" t="s">
         <v>84</v>
       </c>
@@ -11560,40 +11498,40 @@
       </c>
     </row>
     <row r="4" spans="2:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="10" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="6" spans="2:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G6" s="10">
+      <c r="G6" s="9">
         <v>1</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="10" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="7" spans="2:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G7" s="10">
+      <c r="G7" s="9">
         <v>2</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="10" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="8" spans="2:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G8" s="10">
+      <c r="G8" s="9">
         <v>3</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="10" t="s">
         <v>78</v>
       </c>
       <c r="J8" t="s">
@@ -11669,10 +11607,10 @@
       </c>
     </row>
     <row r="9" spans="2:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G9" s="10">
+      <c r="G9" s="9">
         <v>4</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="10" t="s">
         <v>76</v>
       </c>
       <c r="K9" t="s">
@@ -11728,18 +11666,18 @@
       </c>
     </row>
     <row r="10" spans="2:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="10">
+      <c r="G10" s="9">
         <v>5</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="10" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="11" spans="2:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G11" s="10">
+      <c r="G11" s="9">
         <v>6</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="10" t="s">
         <v>76</v>
       </c>
       <c r="J11" t="s">
@@ -11815,10 +11753,10 @@
       </c>
     </row>
     <row r="12" spans="2:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G12" s="10">
+      <c r="G12" s="9">
         <v>7</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="10" t="s">
         <v>78</v>
       </c>
       <c r="K12" t="s">
@@ -11874,26 +11812,26 @@
       </c>
     </row>
     <row r="13" spans="2:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G13" s="10">
+      <c r="G13" s="9">
         <v>8</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="10" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="14" spans="2:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G14" s="10">
+      <c r="G14" s="9">
         <v>9</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="10" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="15" spans="2:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G15" s="10">
+      <c r="G15" s="9">
         <v>10</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="10" t="s">
         <v>76</v>
       </c>
       <c r="J15">
@@ -11904,10 +11842,10 @@
       </c>
     </row>
     <row r="16" spans="2:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G16" s="10">
+      <c r="G16" s="9">
         <v>11</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="10" t="s">
         <v>76</v>
       </c>
       <c r="J16">
@@ -11919,10 +11857,10 @@
       </c>
     </row>
     <row r="17" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G17" s="10">
+      <c r="G17" s="9">
         <v>12</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="10" t="s">
         <v>76</v>
       </c>
       <c r="J17">
@@ -11934,10 +11872,10 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G18" s="10">
+      <c r="G18" s="9">
         <v>13</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="10" t="s">
         <v>78</v>
       </c>
       <c r="J18">
@@ -11949,10 +11887,10 @@
       </c>
     </row>
     <row r="19" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G19" s="10">
+      <c r="G19" s="9">
         <v>14</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="10" t="s">
         <v>76</v>
       </c>
       <c r="J19">
@@ -11964,11 +11902,11 @@
       </c>
     </row>
     <row r="20" spans="2:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="9"/>
-      <c r="G20" s="10">
+      <c r="B20" s="8"/>
+      <c r="G20" s="9">
         <v>15</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="10" t="s">
         <v>76</v>
       </c>
       <c r="J20">
@@ -11980,10 +11918,10 @@
       </c>
     </row>
     <row r="21" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G21" s="11">
+      <c r="G21" s="10">
         <v>16</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="H21" s="10" t="s">
         <v>76</v>
       </c>
       <c r="J21">
@@ -11995,18 +11933,18 @@
       </c>
     </row>
     <row r="22" spans="2:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="86" t="s">
+      <c r="B22" s="78" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="88"/>
-      <c r="D22" s="86" t="s">
+      <c r="C22" s="80"/>
+      <c r="D22" s="78" t="s">
         <v>83</v>
       </c>
-      <c r="E22" s="88"/>
-      <c r="G22" s="11">
+      <c r="E22" s="80"/>
+      <c r="G22" s="10">
         <v>17</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="H22" s="10" t="s">
         <v>78</v>
       </c>
       <c r="J22">
@@ -12018,22 +11956,22 @@
       </c>
     </row>
     <row r="23" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="10">
         <v>18</v>
       </c>
-      <c r="H23" s="11" t="s">
+      <c r="H23" s="10" t="s">
         <v>76</v>
       </c>
       <c r="J23">
@@ -12045,22 +11983,22 @@
       </c>
     </row>
     <row r="24" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="10">
+      <c r="B24" s="9">
         <v>1</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="10">
         <v>1</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G24" s="10">
         <v>19</v>
       </c>
-      <c r="H24" s="11" t="s">
+      <c r="H24" s="10" t="s">
         <v>76</v>
       </c>
       <c r="J24">
@@ -12072,22 +12010,22 @@
       </c>
     </row>
     <row r="25" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="10">
+      <c r="B25" s="9">
         <v>2</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="10">
         <v>2</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G25" s="10">
         <v>20</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="10" t="s">
         <v>78</v>
       </c>
       <c r="J25">
@@ -12099,22 +12037,22 @@
       </c>
     </row>
     <row r="26" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="10">
+      <c r="B26" s="9">
         <v>3</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="10">
         <v>3</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G26" s="10">
         <v>21</v>
       </c>
-      <c r="H26" s="11" t="s">
+      <c r="H26" s="10" t="s">
         <v>78</v>
       </c>
       <c r="J26">
@@ -12126,22 +12064,22 @@
       </c>
     </row>
     <row r="27" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="10">
+      <c r="B27" s="9">
         <v>4</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="10">
         <v>4</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G27" s="10">
         <v>22</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H27" s="10" t="s">
         <v>78</v>
       </c>
       <c r="J27">
@@ -12153,22 +12091,22 @@
       </c>
     </row>
     <row r="28" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="10">
+      <c r="B28" s="9">
         <v>5</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D28" s="10">
         <v>5</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="G28" s="11">
+      <c r="G28" s="10">
         <v>23</v>
       </c>
-      <c r="H28" s="11" t="s">
+      <c r="H28" s="10" t="s">
         <v>74</v>
       </c>
       <c r="J28">
@@ -12180,22 +12118,22 @@
       </c>
     </row>
     <row r="29" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="10">
+      <c r="B29" s="9">
         <v>6</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D29" s="10">
         <v>6</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G29" s="11">
+      <c r="G29" s="10">
         <v>24</v>
       </c>
-      <c r="H29" s="11" t="s">
+      <c r="H29" s="10" t="s">
         <v>76</v>
       </c>
       <c r="J29">
@@ -12207,22 +12145,22 @@
       </c>
     </row>
     <row r="30" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="10">
+      <c r="B30" s="9">
         <v>7</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D30" s="10">
         <v>7</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="G30" s="11">
+      <c r="G30" s="10">
         <v>25</v>
       </c>
-      <c r="H30" s="11" t="s">
+      <c r="H30" s="10" t="s">
         <v>76</v>
       </c>
       <c r="J30">
@@ -12234,22 +12172,22 @@
       </c>
     </row>
     <row r="31" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="10">
+      <c r="B31" s="9">
         <v>8</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="10">
         <v>8</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="G31" s="11">
+      <c r="G31" s="10">
         <v>26</v>
       </c>
-      <c r="H31" s="11" t="s">
+      <c r="H31" s="10" t="s">
         <v>76</v>
       </c>
       <c r="J31">
@@ -12261,22 +12199,22 @@
       </c>
     </row>
     <row r="32" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="10">
+      <c r="B32" s="9">
         <v>9</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D32" s="10">
         <v>9</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="G32" s="11">
+      <c r="G32" s="10">
         <v>27</v>
       </c>
-      <c r="H32" s="11" t="s">
+      <c r="H32" s="10" t="s">
         <v>76</v>
       </c>
       <c r="J32">
@@ -12288,22 +12226,22 @@
       </c>
     </row>
     <row r="33" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="10">
+      <c r="B33" s="9">
         <v>10</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D33" s="10">
         <v>10</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="G33" s="11">
+      <c r="G33" s="10">
         <v>28</v>
       </c>
-      <c r="H33" s="11" t="s">
+      <c r="H33" s="10" t="s">
         <v>74</v>
       </c>
       <c r="J33">
@@ -12315,22 +12253,22 @@
       </c>
     </row>
     <row r="34" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="10">
+      <c r="B34" s="9">
         <v>11</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D34" s="10">
         <v>11</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="E34" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="G34" s="11">
+      <c r="G34" s="10">
         <v>29</v>
       </c>
-      <c r="H34" s="11" t="s">
+      <c r="H34" s="10" t="s">
         <v>76</v>
       </c>
       <c r="J34">
@@ -12342,22 +12280,22 @@
       </c>
     </row>
     <row r="35" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="10">
+      <c r="B35" s="9">
         <v>12</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D35" s="11">
+      <c r="D35" s="10">
         <v>12</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="E35" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="G35" s="11">
+      <c r="G35" s="10">
         <v>30</v>
       </c>
-      <c r="H35" s="11" t="s">
+      <c r="H35" s="10" t="s">
         <v>76</v>
       </c>
       <c r="J35">
@@ -12369,16 +12307,16 @@
       </c>
     </row>
     <row r="36" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="10">
+      <c r="B36" s="9">
         <v>13</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="11">
+      <c r="D36" s="10">
         <v>13</v>
       </c>
-      <c r="E36" s="11" t="s">
+      <c r="E36" s="10" t="s">
         <v>78</v>
       </c>
       <c r="J36">
@@ -12390,16 +12328,16 @@
       </c>
     </row>
     <row r="37" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="10">
+      <c r="B37" s="9">
         <v>14</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D37" s="11">
+      <c r="D37" s="10">
         <v>14</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="10" t="s">
         <v>77</v>
       </c>
       <c r="J37">
@@ -12411,16 +12349,16 @@
       </c>
     </row>
     <row r="38" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="10">
+      <c r="B38" s="9">
         <v>15</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D38" s="11">
+      <c r="D38" s="10">
         <v>15</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="E38" s="10" t="s">
         <v>76</v>
       </c>
       <c r="J38">
@@ -12432,16 +12370,16 @@
       </c>
     </row>
     <row r="39" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="10">
+      <c r="B39" s="9">
         <v>16</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D39" s="11">
+      <c r="D39" s="10">
         <v>16</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="E39" s="10" t="s">
         <v>76</v>
       </c>
       <c r="J39">
@@ -12453,16 +12391,16 @@
       </c>
     </row>
     <row r="40" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="10">
+      <c r="B40" s="9">
         <v>17</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="11">
+      <c r="D40" s="10">
         <v>17</v>
       </c>
-      <c r="E40" s="11" t="s">
+      <c r="E40" s="10" t="s">
         <v>75</v>
       </c>
       <c r="J40">
@@ -12483,55 +12421,55 @@
       </c>
     </row>
     <row r="42" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B42" s="9"/>
+      <c r="B42" s="8"/>
     </row>
     <row r="44" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B44" s="9"/>
+      <c r="B44" s="8"/>
     </row>
     <row r="46" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B46" s="9"/>
+      <c r="B46" s="8"/>
     </row>
     <row r="48" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B48" s="9"/>
+      <c r="B48" s="8"/>
     </row>
     <row r="50" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B50" s="9"/>
+      <c r="B50" s="8"/>
     </row>
     <row r="52" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B52" s="9"/>
+      <c r="B52" s="8"/>
     </row>
     <row r="54" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B54" s="9"/>
+      <c r="B54" s="8"/>
     </row>
     <row r="56" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B56" s="9"/>
+      <c r="B56" s="8"/>
     </row>
     <row r="58" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B58" s="9"/>
+      <c r="B58" s="8"/>
     </row>
     <row r="60" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B60" s="9"/>
+      <c r="B60" s="8"/>
     </row>
     <row r="62" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B62" s="9"/>
+      <c r="B62" s="8"/>
     </row>
     <row r="64" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B64" s="9"/>
+      <c r="B64" s="8"/>
     </row>
     <row r="66" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B66" s="9"/>
+      <c r="B66" s="8"/>
     </row>
     <row r="68" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B68" s="9"/>
+      <c r="B68" s="8"/>
     </row>
     <row r="70" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B70" s="9"/>
+      <c r="B70" s="8"/>
     </row>
     <row r="72" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B72" s="9"/>
+      <c r="B72" s="8"/>
     </row>
     <row r="74" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B74" s="9"/>
+      <c r="B74" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
DAT_RA y DAT_RM con imagenes nuevas y otros cambios
</commit_message>
<xml_diff>
--- a/DAT/Exportar/Documento_Modelo/Base_de_Datos.xlsx
+++ b/DAT/Exportar/Documento_Modelo/Base_de_Datos.xlsx
@@ -573,9 +573,6 @@
     <t>TR no incluye el tiempo de lectura de la consigna o el tiempo de la práctica en Bloques de Corsi</t>
   </si>
   <si>
-    <t>TIEMPOS DE REACCIÓN</t>
-  </si>
-  <si>
     <t>Serie_CS</t>
   </si>
   <si>
@@ -598,6 +595,9 @@
   </si>
   <si>
     <t>Tiempo Total</t>
+  </si>
+  <si>
+    <t>TIEMPOS DE REACCIÓN (ms)</t>
   </si>
 </sst>
 </file>
@@ -1412,6 +1412,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1459,12 +1465,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9534,10 +9534,10 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -9722,10 +9722,10 @@
   <dimension ref="A1:CT9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="CM4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="CH4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="CS14" sqref="CS14"/>
+      <selection pane="bottomRight" activeCell="CS12" sqref="CS12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -9848,41 +9848,41 @@
       <c r="BU1" s="21"/>
       <c r="BV1" s="21"/>
       <c r="BW1" s="23"/>
-      <c r="BX1" s="69" t="s">
+      <c r="BX1" s="71" t="s">
         <v>182</v>
       </c>
-      <c r="BY1" s="70" t="s">
+      <c r="BY1" s="72" t="s">
         <v>183</v>
       </c>
       <c r="BZ1" s="17"/>
-      <c r="CA1" s="71" t="s">
+      <c r="CA1" s="73" t="s">
         <v>181</v>
       </c>
-      <c r="CB1" s="72"/>
-      <c r="CC1" s="72"/>
-      <c r="CD1" s="72"/>
-      <c r="CE1" s="73"/>
-      <c r="CF1" s="73"/>
-      <c r="CG1" s="74"/>
-      <c r="CH1" s="71" t="s">
-        <v>190</v>
-      </c>
-      <c r="CI1" s="72"/>
-      <c r="CJ1" s="72"/>
-      <c r="CK1" s="72"/>
-      <c r="CL1" s="73"/>
-      <c r="CM1" s="73"/>
-      <c r="CN1" s="75" t="s">
-        <v>185</v>
-      </c>
-      <c r="CO1" s="76"/>
-      <c r="CP1" s="76"/>
-      <c r="CQ1" s="76"/>
-      <c r="CR1" s="77"/>
-      <c r="CS1" s="65" t="s">
+      <c r="CB1" s="74"/>
+      <c r="CC1" s="74"/>
+      <c r="CD1" s="74"/>
+      <c r="CE1" s="75"/>
+      <c r="CF1" s="75"/>
+      <c r="CG1" s="76"/>
+      <c r="CH1" s="73" t="s">
+        <v>189</v>
+      </c>
+      <c r="CI1" s="74"/>
+      <c r="CJ1" s="74"/>
+      <c r="CK1" s="74"/>
+      <c r="CL1" s="75"/>
+      <c r="CM1" s="75"/>
+      <c r="CN1" s="77" t="s">
+        <v>193</v>
+      </c>
+      <c r="CO1" s="78"/>
+      <c r="CP1" s="78"/>
+      <c r="CQ1" s="78"/>
+      <c r="CR1" s="79"/>
+      <c r="CS1" s="67" t="s">
         <v>184</v>
       </c>
-      <c r="CT1" s="66"/>
+      <c r="CT1" s="68"/>
     </row>
     <row r="2" spans="1:98" s="11" customFormat="1" ht="78.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
@@ -10088,8 +10088,8 @@
       <c r="BW2" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="BX2" s="69"/>
-      <c r="BY2" s="70"/>
+      <c r="BX2" s="71"/>
+      <c r="BY2" s="72"/>
       <c r="BZ2" s="16"/>
       <c r="CA2" s="40" t="s">
         <v>173</v>
@@ -10104,16 +10104,16 @@
         <v>176</v>
       </c>
       <c r="CE2" s="42" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="CF2" s="42" t="s">
         <v>177</v>
       </c>
       <c r="CG2" s="47" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="CH2" s="61" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="CI2" s="59"/>
       <c r="CJ2" s="59"/>
@@ -10129,12 +10129,12 @@
       <c r="CP2" s="44" t="s">
         <v>178</v>
       </c>
-      <c r="CQ2" s="67" t="s">
+      <c r="CQ2" s="69" t="s">
         <v>180</v>
       </c>
-      <c r="CR2" s="68"/>
-      <c r="CS2" s="65"/>
-      <c r="CT2" s="66"/>
+      <c r="CR2" s="70"/>
+      <c r="CS2" s="67"/>
+      <c r="CT2" s="68"/>
     </row>
     <row r="3" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
@@ -10170,7 +10170,7 @@
       <c r="K3" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="L3" s="81" t="s">
+      <c r="L3" s="65" t="s">
         <v>7</v>
       </c>
       <c r="M3" s="15" t="s">
@@ -10221,7 +10221,7 @@
       <c r="AB3" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="AC3" s="81" t="s">
+      <c r="AC3" s="65" t="s">
         <v>24</v>
       </c>
       <c r="AD3" s="15" t="s">
@@ -10311,7 +10311,7 @@
       <c r="BF3" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="BG3" s="81" t="s">
+      <c r="BG3" s="65" t="s">
         <v>54</v>
       </c>
       <c r="BH3" s="15" t="s">
@@ -10362,7 +10362,7 @@
       <c r="BW3" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="BX3" s="81" t="s">
+      <c r="BX3" s="65" t="s">
         <v>156</v>
       </c>
       <c r="BY3" s="19" t="s">
@@ -10371,7 +10371,7 @@
       <c r="BZ3" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="CA3" s="81" t="s">
+      <c r="CA3" s="65" t="s">
         <v>115</v>
       </c>
       <c r="CB3" s="15" t="s">
@@ -10384,13 +10384,13 @@
         <v>158</v>
       </c>
       <c r="CE3" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="CF3" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="CG3" s="82" t="s">
-        <v>187</v>
+      <c r="CG3" s="66" t="s">
+        <v>186</v>
       </c>
       <c r="CH3" s="15" t="s">
         <v>167</v>
@@ -10426,7 +10426,7 @@
         <v>161</v>
       </c>
       <c r="CS3" s="19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="CT3" s="19" t="s">
         <v>151</v>
@@ -11400,12 +11400,12 @@
       </c>
     </row>
     <row r="3" spans="2:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="80"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="82"/>
       <c r="I3" t="s">
         <v>84</v>
       </c>
@@ -11933,14 +11933,14 @@
       </c>
     </row>
     <row r="22" spans="2:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="78" t="s">
+      <c r="B22" s="80" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="80"/>
-      <c r="D22" s="78" t="s">
+      <c r="C22" s="82"/>
+      <c r="D22" s="80" t="s">
         <v>83</v>
       </c>
-      <c r="E22" s="80"/>
+      <c r="E22" s="82"/>
       <c r="G22" s="10">
         <v>17</v>
       </c>

</xml_diff>